<commit_message>
Create and complete r17.py
</commit_message>
<xml_diff>
--- a/crisis_src/crisis_sfy_2021.xlsx
+++ b/crisis_src/crisis_sfy_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KHIT docs\KHIT-scripts\crisis_src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C570BCDD-2753-4671-8070-81B111E1AB9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDA99DE5-0BCE-4298-9658-ED6689269CE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="690" yWindow="4080" windowWidth="21585" windowHeight="11805" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="crisis_src" sheetId="1" r:id="rId1"/>
@@ -696,7 +696,7 @@
   <dimension ref="A1:X75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18:L19"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
r17.py: Script marked as completed
</commit_message>
<xml_diff>
--- a/crisis_src/crisis_sfy_2021.xlsx
+++ b/crisis_src/crisis_sfy_2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KHIT docs\KHIT-scripts\crisis_src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDA99DE5-0BCE-4298-9658-ED6689269CE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{304785CF-E6C4-4B64-9A18-2BE40F83FFB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="690" yWindow="4080" windowWidth="21585" windowHeight="11805" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2085" yWindow="1740" windowWidth="21585" windowHeight="11805" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="crisis_src" sheetId="1" r:id="rId1"/>
@@ -695,8 +695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
r21.py: Script marked as completed
</commit_message>
<xml_diff>
--- a/crisis_src/crisis_sfy_2021.xlsx
+++ b/crisis_src/crisis_sfy_2021.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KHIT docs\KHIT-scripts\crisis_src\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{304785CF-E6C4-4B64-9A18-2BE40F83FFB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2085" yWindow="1740" windowWidth="21585" windowHeight="11805" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="crisis_src" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -297,8 +291,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -361,14 +355,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -415,7 +401,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -447,27 +433,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -499,24 +467,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -692,16 +642,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -775,7 +723,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24">
       <c r="C2">
         <v>2</v>
       </c>
@@ -822,7 +770,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24">
       <c r="B3" t="s">
         <v>27</v>
       </c>
@@ -872,7 +820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24">
       <c r="C4">
         <v>4</v>
       </c>
@@ -919,7 +867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24">
       <c r="C5">
         <v>5</v>
       </c>
@@ -966,7 +914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24">
       <c r="C6">
         <v>6</v>
       </c>
@@ -1016,7 +964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24">
       <c r="C7">
         <v>7</v>
       </c>
@@ -1066,7 +1014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24">
       <c r="C8">
         <v>8</v>
       </c>
@@ -1116,7 +1064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24">
       <c r="C9">
         <v>9</v>
       </c>
@@ -1166,7 +1114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24">
       <c r="C10">
         <v>10</v>
       </c>
@@ -1216,7 +1164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24">
       <c r="C11">
         <v>11</v>
       </c>
@@ -1266,7 +1214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24">
       <c r="C12">
         <v>12</v>
       </c>
@@ -1316,7 +1264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24">
       <c r="C13">
         <v>13</v>
       </c>
@@ -1366,7 +1314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24">
       <c r="C14">
         <v>14</v>
       </c>
@@ -1416,7 +1364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24">
       <c r="C15">
         <v>15</v>
       </c>
@@ -1466,7 +1414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24">
       <c r="C16">
         <v>16</v>
       </c>
@@ -1516,7 +1464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20">
       <c r="C17">
         <v>17</v>
       </c>
@@ -1530,7 +1478,7 @@
         <v>0</v>
       </c>
       <c r="G17">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="H17">
         <v>0</v>
@@ -1560,13 +1508,13 @@
         <v>0</v>
       </c>
       <c r="Q17">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="R17">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20">
       <c r="B18" t="s">
         <v>28</v>
       </c>
@@ -1622,7 +1570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20">
       <c r="C19">
         <v>19</v>
       </c>
@@ -1672,7 +1620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20">
       <c r="C20">
         <v>20</v>
       </c>
@@ -1722,7 +1670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20">
       <c r="B21" t="s">
         <v>29</v>
       </c>
@@ -1739,7 +1687,7 @@
         <v>0</v>
       </c>
       <c r="G21">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="H21">
         <v>0</v>
@@ -1769,13 +1717,13 @@
         <v>0</v>
       </c>
       <c r="Q21">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="R21">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20">
       <c r="C22">
         <v>22</v>
       </c>
@@ -1825,7 +1773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20">
       <c r="C23">
         <v>23</v>
       </c>
@@ -1875,7 +1823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20">
       <c r="C24">
         <v>24</v>
       </c>
@@ -1925,7 +1873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20">
       <c r="C25">
         <v>25</v>
       </c>
@@ -1975,7 +1923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20">
       <c r="C26">
         <v>26</v>
       </c>
@@ -2025,7 +1973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20">
       <c r="C27">
         <v>27</v>
       </c>
@@ -2075,7 +2023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20">
       <c r="C28">
         <v>28</v>
       </c>
@@ -2125,7 +2073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20">
       <c r="C29">
         <v>29</v>
       </c>
@@ -2175,7 +2123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20">
       <c r="A30" t="s">
         <v>24</v>
       </c>
@@ -2228,7 +2176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20">
       <c r="C31">
         <v>31</v>
       </c>
@@ -2278,7 +2226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20">
       <c r="C32">
         <v>32</v>
       </c>
@@ -2328,7 +2276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:20">
       <c r="C33">
         <v>33</v>
       </c>
@@ -2378,7 +2326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:20">
       <c r="C34">
         <v>34</v>
       </c>
@@ -2428,7 +2376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:20">
       <c r="C35">
         <v>35</v>
       </c>
@@ -2478,7 +2426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:20">
       <c r="C36">
         <v>36</v>
       </c>
@@ -2528,7 +2476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:20">
       <c r="C37">
         <v>37</v>
       </c>
@@ -2578,7 +2526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:20">
       <c r="C38">
         <v>38</v>
       </c>
@@ -2628,7 +2576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:20">
       <c r="C39">
         <v>39</v>
       </c>
@@ -2678,7 +2626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:20">
       <c r="C40">
         <v>40</v>
       </c>
@@ -2728,7 +2676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:20">
       <c r="C41">
         <v>41</v>
       </c>
@@ -2778,7 +2726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:20">
       <c r="C42">
         <v>42</v>
       </c>
@@ -2828,7 +2776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:20">
       <c r="C43">
         <v>43</v>
       </c>
@@ -2878,7 +2826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:20">
       <c r="C44">
         <v>44</v>
       </c>
@@ -2928,7 +2876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:20">
       <c r="C45">
         <v>45</v>
       </c>
@@ -2978,7 +2926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:20">
       <c r="C46">
         <v>46</v>
       </c>
@@ -3028,7 +2976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:20">
       <c r="C47">
         <v>47</v>
       </c>
@@ -3078,7 +3026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:20">
       <c r="C48">
         <v>48</v>
       </c>
@@ -3128,7 +3076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:24">
       <c r="A49" t="s">
         <v>25</v>
       </c>
@@ -3190,7 +3138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:24">
       <c r="C50">
         <v>50</v>
       </c>
@@ -3243,7 +3191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:24">
       <c r="C51">
         <v>51</v>
       </c>
@@ -3296,7 +3244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:24">
       <c r="C52">
         <v>52</v>
       </c>
@@ -3349,7 +3297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:24">
       <c r="C53">
         <v>53</v>
       </c>
@@ -3402,7 +3350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:24">
       <c r="C54">
         <v>54</v>
       </c>
@@ -3452,7 +3400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:24">
       <c r="B55" t="s">
         <v>31</v>
       </c>
@@ -3511,7 +3459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:24">
       <c r="C56">
         <v>56</v>
       </c>
@@ -3564,7 +3512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:24">
       <c r="C57">
         <v>57</v>
       </c>
@@ -3617,7 +3565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:24">
       <c r="C58">
         <v>58</v>
       </c>
@@ -3670,7 +3618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:24">
       <c r="C59">
         <v>59</v>
       </c>
@@ -3723,7 +3671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:24">
       <c r="C60">
         <v>60</v>
       </c>
@@ -3776,7 +3724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:24">
       <c r="C61">
         <v>61</v>
       </c>
@@ -3829,7 +3777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:24">
       <c r="C62">
         <v>62</v>
       </c>
@@ -3882,7 +3830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:24">
       <c r="C63">
         <v>63</v>
       </c>
@@ -3935,7 +3883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:24">
       <c r="C64">
         <v>64</v>
       </c>
@@ -3988,7 +3936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:23">
       <c r="C65">
         <v>65</v>
       </c>
@@ -4041,7 +3989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:23">
       <c r="C66">
         <v>66</v>
       </c>
@@ -4094,7 +4042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:23">
       <c r="C67">
         <v>67</v>
       </c>
@@ -4147,7 +4095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:23">
       <c r="C68">
         <v>68</v>
       </c>
@@ -4200,7 +4148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:23">
       <c r="C69">
         <v>69</v>
       </c>
@@ -4253,7 +4201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:23">
       <c r="C70">
         <v>70</v>
       </c>
@@ -4306,7 +4254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:23">
       <c r="C71">
         <v>71</v>
       </c>
@@ -4359,7 +4307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:23">
       <c r="C72">
         <v>72</v>
       </c>
@@ -4412,7 +4360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:23">
       <c r="C73">
         <v>73</v>
       </c>
@@ -4465,7 +4413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:23">
       <c r="C74">
         <v>74</v>
       </c>
@@ -4515,7 +4463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:23">
       <c r="A75" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
r27.py: Script created and marked as complete
</commit_message>
<xml_diff>
--- a/crisis_src/crisis_sfy_2021.xlsx
+++ b/crisis_src/crisis_sfy_2021.xlsx
@@ -1987,7 +1987,7 @@
         <v>0</v>
       </c>
       <c r="G27">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="H27">
         <v>0</v>
@@ -2017,7 +2017,7 @@
         <v>0</v>
       </c>
       <c r="Q27">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="R27">
         <v>0</v>

</xml_diff>

<commit_message>
r18-20.py: Script marked as completed
</commit_message>
<xml_diff>
--- a/crisis_src/crisis_sfy_2021.xlsx
+++ b/crisis_src/crisis_sfy_2021.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KHIT docs\KHIT-scripts\crisis_src\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBDE4474-B9C8-452D-855B-FF42593B1E01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="6360" yWindow="2415" windowWidth="21585" windowHeight="11805" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="crisis_src" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -291,8 +297,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -355,6 +361,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -401,7 +415,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -433,9 +447,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -467,6 +499,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -642,14 +692,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -723,7 +775,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C2">
         <v>2</v>
       </c>
@@ -770,7 +822,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>27</v>
       </c>
@@ -820,7 +872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>4</v>
       </c>
@@ -867,7 +919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>5</v>
       </c>
@@ -914,7 +966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>6</v>
       </c>
@@ -964,7 +1016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>7</v>
       </c>
@@ -1014,7 +1066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>8</v>
       </c>
@@ -1064,7 +1116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>9</v>
       </c>
@@ -1114,7 +1166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C10">
         <v>10</v>
       </c>
@@ -1164,7 +1216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:24">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>11</v>
       </c>
@@ -1214,7 +1266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:24">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C12">
         <v>12</v>
       </c>
@@ -1264,7 +1316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:24">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C13">
         <v>13</v>
       </c>
@@ -1314,7 +1366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:24">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C14">
         <v>14</v>
       </c>
@@ -1364,7 +1416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:24">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C15">
         <v>15</v>
       </c>
@@ -1414,7 +1466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:24">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C16">
         <v>16</v>
       </c>
@@ -1464,7 +1516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C17">
         <v>17</v>
       </c>
@@ -1514,7 +1566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>28</v>
       </c>
@@ -1531,7 +1583,7 @@
         <v>0</v>
       </c>
       <c r="G18">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="H18">
         <v>0</v>
@@ -1561,7 +1613,7 @@
         <v>0</v>
       </c>
       <c r="Q18">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="R18">
         <v>0</v>
@@ -1570,7 +1622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:20">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C19">
         <v>19</v>
       </c>
@@ -1584,7 +1636,7 @@
         <v>0</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -1614,13 +1666,13 @@
         <v>0</v>
       </c>
       <c r="Q19">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R19">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:20">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C20">
         <v>20</v>
       </c>
@@ -1634,7 +1686,7 @@
         <v>0</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -1664,13 +1716,13 @@
         <v>0</v>
       </c>
       <c r="Q20">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R20">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>29</v>
       </c>
@@ -1723,7 +1775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:20">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C22">
         <v>22</v>
       </c>
@@ -1773,7 +1825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:20">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>23</v>
       </c>
@@ -1823,7 +1875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:20">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C24">
         <v>24</v>
       </c>
@@ -1873,7 +1925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:20">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C25">
         <v>25</v>
       </c>
@@ -1923,7 +1975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:20">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C26">
         <v>26</v>
       </c>
@@ -1973,7 +2025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:20">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C27">
         <v>27</v>
       </c>
@@ -2023,7 +2075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:20">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C28">
         <v>28</v>
       </c>
@@ -2073,7 +2125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:20">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C29">
         <v>29</v>
       </c>
@@ -2123,7 +2175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:20">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>24</v>
       </c>
@@ -2176,7 +2228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:20">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C31">
         <v>31</v>
       </c>
@@ -2226,7 +2278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:20">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C32">
         <v>32</v>
       </c>
@@ -2276,7 +2328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="3:20">
+    <row r="33" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C33">
         <v>33</v>
       </c>
@@ -2326,7 +2378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="3:20">
+    <row r="34" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C34">
         <v>34</v>
       </c>
@@ -2376,7 +2428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="3:20">
+    <row r="35" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C35">
         <v>35</v>
       </c>
@@ -2426,7 +2478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="3:20">
+    <row r="36" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C36">
         <v>36</v>
       </c>
@@ -2476,7 +2528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="3:20">
+    <row r="37" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C37">
         <v>37</v>
       </c>
@@ -2526,7 +2578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="3:20">
+    <row r="38" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C38">
         <v>38</v>
       </c>
@@ -2576,7 +2628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="3:20">
+    <row r="39" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C39">
         <v>39</v>
       </c>
@@ -2626,7 +2678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="3:20">
+    <row r="40" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C40">
         <v>40</v>
       </c>
@@ -2676,7 +2728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="3:20">
+    <row r="41" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C41">
         <v>41</v>
       </c>
@@ -2726,7 +2778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="3:20">
+    <row r="42" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C42">
         <v>42</v>
       </c>
@@ -2776,7 +2828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="3:20">
+    <row r="43" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C43">
         <v>43</v>
       </c>
@@ -2826,7 +2878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="3:20">
+    <row r="44" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C44">
         <v>44</v>
       </c>
@@ -2876,7 +2928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="3:20">
+    <row r="45" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C45">
         <v>45</v>
       </c>
@@ -2926,7 +2978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="3:20">
+    <row r="46" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C46">
         <v>46</v>
       </c>
@@ -2976,7 +3028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="3:20">
+    <row r="47" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C47">
         <v>47</v>
       </c>
@@ -3026,7 +3078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="3:20">
+    <row r="48" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C48">
         <v>48</v>
       </c>
@@ -3076,7 +3128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:24">
+    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>25</v>
       </c>
@@ -3138,7 +3190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:24">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C50">
         <v>50</v>
       </c>
@@ -3191,7 +3243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:24">
+    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C51">
         <v>51</v>
       </c>
@@ -3244,7 +3296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:24">
+    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C52">
         <v>52</v>
       </c>
@@ -3297,7 +3349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:24">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C53">
         <v>53</v>
       </c>
@@ -3350,7 +3402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:24">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C54">
         <v>54</v>
       </c>
@@ -3400,7 +3452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:24">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>31</v>
       </c>
@@ -3459,7 +3511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:24">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C56">
         <v>56</v>
       </c>
@@ -3512,7 +3564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:24">
+    <row r="57" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C57">
         <v>57</v>
       </c>
@@ -3565,7 +3617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:24">
+    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C58">
         <v>58</v>
       </c>
@@ -3618,7 +3670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:24">
+    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C59">
         <v>59</v>
       </c>
@@ -3671,7 +3723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:24">
+    <row r="60" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C60">
         <v>60</v>
       </c>
@@ -3724,7 +3776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:24">
+    <row r="61" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C61">
         <v>61</v>
       </c>
@@ -3777,7 +3829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:24">
+    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C62">
         <v>62</v>
       </c>
@@ -3830,7 +3882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:24">
+    <row r="63" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C63">
         <v>63</v>
       </c>
@@ -3883,7 +3935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:24">
+    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C64">
         <v>64</v>
       </c>
@@ -3936,7 +3988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:23">
+    <row r="65" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C65">
         <v>65</v>
       </c>
@@ -3989,7 +4041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:23">
+    <row r="66" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C66">
         <v>66</v>
       </c>
@@ -4042,7 +4094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:23">
+    <row r="67" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C67">
         <v>67</v>
       </c>
@@ -4095,7 +4147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:23">
+    <row r="68" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C68">
         <v>68</v>
       </c>
@@ -4148,7 +4200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:23">
+    <row r="69" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C69">
         <v>69</v>
       </c>
@@ -4201,7 +4253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:23">
+    <row r="70" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C70">
         <v>70</v>
       </c>
@@ -4254,7 +4306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:23">
+    <row r="71" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C71">
         <v>71</v>
       </c>
@@ -4307,7 +4359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:23">
+    <row r="72" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C72">
         <v>72</v>
       </c>
@@ -4360,7 +4412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:23">
+    <row r="73" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C73">
         <v>73</v>
       </c>
@@ -4413,7 +4465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:23">
+    <row r="74" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C74">
         <v>74</v>
       </c>
@@ -4463,7 +4515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:23">
+    <row r="75" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
r28-29.py: Script marked as complete
</commit_message>
<xml_diff>
--- a/crisis_src/crisis_sfy_2021.xlsx
+++ b/crisis_src/crisis_sfy_2021.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KHIT docs\KHIT-scripts\crisis_src\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBDE4474-B9C8-452D-855B-FF42593B1E01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6360" yWindow="2415" windowWidth="21585" windowHeight="11805" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="crisis_src" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -297,8 +291,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -361,14 +355,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -415,7 +401,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -447,27 +433,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -499,24 +467,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -692,16 +642,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -775,7 +723,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24">
       <c r="C2">
         <v>2</v>
       </c>
@@ -822,7 +770,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24">
       <c r="B3" t="s">
         <v>27</v>
       </c>
@@ -872,7 +820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24">
       <c r="C4">
         <v>4</v>
       </c>
@@ -919,7 +867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24">
       <c r="C5">
         <v>5</v>
       </c>
@@ -966,7 +914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24">
       <c r="C6">
         <v>6</v>
       </c>
@@ -1016,7 +964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24">
       <c r="C7">
         <v>7</v>
       </c>
@@ -1066,7 +1014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24">
       <c r="C8">
         <v>8</v>
       </c>
@@ -1116,7 +1064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24">
       <c r="C9">
         <v>9</v>
       </c>
@@ -1166,7 +1114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24">
       <c r="C10">
         <v>10</v>
       </c>
@@ -1216,7 +1164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24">
       <c r="C11">
         <v>11</v>
       </c>
@@ -1266,7 +1214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24">
       <c r="C12">
         <v>12</v>
       </c>
@@ -1316,7 +1264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24">
       <c r="C13">
         <v>13</v>
       </c>
@@ -1366,7 +1314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24">
       <c r="C14">
         <v>14</v>
       </c>
@@ -1416,7 +1364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24">
       <c r="C15">
         <v>15</v>
       </c>
@@ -1466,7 +1414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24">
       <c r="C16">
         <v>16</v>
       </c>
@@ -1516,7 +1464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20">
       <c r="C17">
         <v>17</v>
       </c>
@@ -1566,7 +1514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20">
       <c r="B18" t="s">
         <v>28</v>
       </c>
@@ -1622,7 +1570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20">
       <c r="C19">
         <v>19</v>
       </c>
@@ -1672,7 +1620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20">
       <c r="C20">
         <v>20</v>
       </c>
@@ -1722,7 +1670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20">
       <c r="B21" t="s">
         <v>29</v>
       </c>
@@ -1775,7 +1723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20">
       <c r="C22">
         <v>22</v>
       </c>
@@ -1825,7 +1773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20">
       <c r="C23">
         <v>23</v>
       </c>
@@ -1875,7 +1823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20">
       <c r="C24">
         <v>24</v>
       </c>
@@ -1925,7 +1873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20">
       <c r="C25">
         <v>25</v>
       </c>
@@ -1975,7 +1923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20">
       <c r="C26">
         <v>26</v>
       </c>
@@ -2025,7 +1973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20">
       <c r="C27">
         <v>27</v>
       </c>
@@ -2075,7 +2023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20">
       <c r="C28">
         <v>28</v>
       </c>
@@ -2125,7 +2073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20">
       <c r="C29">
         <v>29</v>
       </c>
@@ -2175,7 +2123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20">
       <c r="A30" t="s">
         <v>24</v>
       </c>
@@ -2228,7 +2176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20">
       <c r="C31">
         <v>31</v>
       </c>
@@ -2278,7 +2226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20">
       <c r="C32">
         <v>32</v>
       </c>
@@ -2328,7 +2276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:20">
       <c r="C33">
         <v>33</v>
       </c>
@@ -2378,7 +2326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:20">
       <c r="C34">
         <v>34</v>
       </c>
@@ -2428,7 +2376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:20">
       <c r="C35">
         <v>35</v>
       </c>
@@ -2478,7 +2426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:20">
       <c r="C36">
         <v>36</v>
       </c>
@@ -2528,7 +2476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:20">
       <c r="C37">
         <v>37</v>
       </c>
@@ -2578,7 +2526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:20">
       <c r="C38">
         <v>38</v>
       </c>
@@ -2628,7 +2576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:20">
       <c r="C39">
         <v>39</v>
       </c>
@@ -2678,7 +2626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:20">
       <c r="C40">
         <v>40</v>
       </c>
@@ -2728,7 +2676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:20">
       <c r="C41">
         <v>41</v>
       </c>
@@ -2778,7 +2726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:20">
       <c r="C42">
         <v>42</v>
       </c>
@@ -2828,7 +2776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:20">
       <c r="C43">
         <v>43</v>
       </c>
@@ -2878,7 +2826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:20">
       <c r="C44">
         <v>44</v>
       </c>
@@ -2928,7 +2876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:20">
       <c r="C45">
         <v>45</v>
       </c>
@@ -2978,7 +2926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:20">
       <c r="C46">
         <v>46</v>
       </c>
@@ -3028,7 +2976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:20">
       <c r="C47">
         <v>47</v>
       </c>
@@ -3078,7 +3026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:20">
       <c r="C48">
         <v>48</v>
       </c>
@@ -3128,7 +3076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:24">
       <c r="A49" t="s">
         <v>25</v>
       </c>
@@ -3190,7 +3138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:24">
       <c r="C50">
         <v>50</v>
       </c>
@@ -3243,7 +3191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:24">
       <c r="C51">
         <v>51</v>
       </c>
@@ -3296,7 +3244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:24">
       <c r="C52">
         <v>52</v>
       </c>
@@ -3349,7 +3297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:24">
       <c r="C53">
         <v>53</v>
       </c>
@@ -3402,7 +3350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:24">
       <c r="C54">
         <v>54</v>
       </c>
@@ -3452,7 +3400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:24">
       <c r="B55" t="s">
         <v>31</v>
       </c>
@@ -3511,7 +3459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:24">
       <c r="C56">
         <v>56</v>
       </c>
@@ -3564,7 +3512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:24">
       <c r="C57">
         <v>57</v>
       </c>
@@ -3617,7 +3565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:24">
       <c r="C58">
         <v>58</v>
       </c>
@@ -3670,7 +3618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:24">
       <c r="C59">
         <v>59</v>
       </c>
@@ -3723,7 +3671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:24">
       <c r="C60">
         <v>60</v>
       </c>
@@ -3776,7 +3724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:24">
       <c r="C61">
         <v>61</v>
       </c>
@@ -3829,7 +3777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:24">
       <c r="C62">
         <v>62</v>
       </c>
@@ -3882,7 +3830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:24">
       <c r="C63">
         <v>63</v>
       </c>
@@ -3935,7 +3883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:24">
       <c r="C64">
         <v>64</v>
       </c>
@@ -3988,7 +3936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:23">
       <c r="C65">
         <v>65</v>
       </c>
@@ -4041,7 +3989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:23">
       <c r="C66">
         <v>66</v>
       </c>
@@ -4094,7 +4042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:23">
       <c r="C67">
         <v>67</v>
       </c>
@@ -4147,7 +4095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:23">
       <c r="C68">
         <v>68</v>
       </c>
@@ -4200,7 +4148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:23">
       <c r="C69">
         <v>69</v>
       </c>
@@ -4253,7 +4201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:23">
       <c r="C70">
         <v>70</v>
       </c>
@@ -4306,7 +4254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:23">
       <c r="C71">
         <v>71</v>
       </c>
@@ -4359,7 +4307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:23">
       <c r="C72">
         <v>72</v>
       </c>
@@ -4412,7 +4360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:23">
       <c r="C73">
         <v>73</v>
       </c>
@@ -4465,7 +4413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:23">
       <c r="C74">
         <v>74</v>
       </c>
@@ -4515,7 +4463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:23">
       <c r="A75" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
r30-48.py: Script marked as complete
</commit_message>
<xml_diff>
--- a/crisis_src/crisis_sfy_2021.xlsx
+++ b/crisis_src/crisis_sfy_2021.xlsx
@@ -2017,7 +2017,7 @@
         <v>0</v>
       </c>
       <c r="Q27">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="R27">
         <v>0</v>
@@ -2190,7 +2190,7 @@
         <v>0</v>
       </c>
       <c r="G31">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H31">
         <v>0</v>
@@ -2220,7 +2220,7 @@
         <v>0</v>
       </c>
       <c r="Q31">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="T31">
         <v>0</v>
@@ -2240,7 +2240,7 @@
         <v>0</v>
       </c>
       <c r="G32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H32">
         <v>0</v>
@@ -2270,7 +2270,7 @@
         <v>0</v>
       </c>
       <c r="Q32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T32">
         <v>0</v>
@@ -2440,7 +2440,7 @@
         <v>0</v>
       </c>
       <c r="G36">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H36">
         <v>0</v>
@@ -2470,7 +2470,7 @@
         <v>0</v>
       </c>
       <c r="Q36">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="T36">
         <v>0</v>
@@ -2540,7 +2540,7 @@
         <v>0</v>
       </c>
       <c r="G38">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H38">
         <v>0</v>
@@ -2570,7 +2570,7 @@
         <v>0</v>
       </c>
       <c r="Q38">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T38">
         <v>0</v>
@@ -2690,7 +2690,7 @@
         <v>0</v>
       </c>
       <c r="G41">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H41">
         <v>0</v>
@@ -2720,7 +2720,7 @@
         <v>0</v>
       </c>
       <c r="Q41">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="T41">
         <v>0</v>
@@ -2990,7 +2990,7 @@
         <v>0</v>
       </c>
       <c r="G47">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H47">
         <v>0</v>
@@ -3020,7 +3020,7 @@
         <v>0</v>
       </c>
       <c r="Q47">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="T47">
         <v>0</v>

</xml_diff>

<commit_message>
r49-73.py: Create script -- finish hospital categorization later
</commit_message>
<xml_diff>
--- a/crisis_src/crisis_sfy_2021.xlsx
+++ b/crisis_src/crisis_sfy_2021.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KHIT docs\KHIT-scripts\crisis_src\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57DF0DDA-8C70-4E0F-8EA3-20FE03F9FC60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21585" windowHeight="11805" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="crisis_src" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -291,8 +297,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -355,6 +361,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -401,7 +415,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -433,9 +447,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -467,6 +499,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -642,14 +692,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="I71" sqref="I71"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -723,7 +775,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C2">
         <v>2</v>
       </c>
@@ -770,7 +822,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>27</v>
       </c>
@@ -820,7 +872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>4</v>
       </c>
@@ -867,7 +919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>5</v>
       </c>
@@ -914,7 +966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>6</v>
       </c>
@@ -964,7 +1016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>7</v>
       </c>
@@ -1014,7 +1066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>8</v>
       </c>
@@ -1064,7 +1116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>9</v>
       </c>
@@ -1114,7 +1166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C10">
         <v>10</v>
       </c>
@@ -1164,7 +1216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:24">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>11</v>
       </c>
@@ -1214,7 +1266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:24">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C12">
         <v>12</v>
       </c>
@@ -1264,7 +1316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:24">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C13">
         <v>13</v>
       </c>
@@ -1314,7 +1366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:24">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C14">
         <v>14</v>
       </c>
@@ -1364,7 +1416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:24">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C15">
         <v>15</v>
       </c>
@@ -1414,7 +1466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:24">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C16">
         <v>16</v>
       </c>
@@ -1464,7 +1516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C17">
         <v>17</v>
       </c>
@@ -1514,7 +1566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>28</v>
       </c>
@@ -1570,7 +1622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:20">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C19">
         <v>19</v>
       </c>
@@ -1620,7 +1672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:20">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C20">
         <v>20</v>
       </c>
@@ -1670,7 +1722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>29</v>
       </c>
@@ -1723,7 +1775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:20">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C22">
         <v>22</v>
       </c>
@@ -1773,7 +1825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:20">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>23</v>
       </c>
@@ -1823,7 +1875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:20">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C24">
         <v>24</v>
       </c>
@@ -1873,7 +1925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:20">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C25">
         <v>25</v>
       </c>
@@ -1923,7 +1975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:20">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C26">
         <v>26</v>
       </c>
@@ -1973,7 +2025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:20">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C27">
         <v>27</v>
       </c>
@@ -2023,7 +2075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:20">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C28">
         <v>28</v>
       </c>
@@ -2073,7 +2125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:20">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C29">
         <v>29</v>
       </c>
@@ -2123,7 +2175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:20">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>24</v>
       </c>
@@ -2176,7 +2228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:20">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C31">
         <v>31</v>
       </c>
@@ -2226,7 +2278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:20">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C32">
         <v>32</v>
       </c>
@@ -2276,7 +2328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="3:20">
+    <row r="33" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C33">
         <v>33</v>
       </c>
@@ -2326,7 +2378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="3:20">
+    <row r="34" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C34">
         <v>34</v>
       </c>
@@ -2376,7 +2428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="3:20">
+    <row r="35" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C35">
         <v>35</v>
       </c>
@@ -2426,7 +2478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="3:20">
+    <row r="36" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C36">
         <v>36</v>
       </c>
@@ -2476,7 +2528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="3:20">
+    <row r="37" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C37">
         <v>37</v>
       </c>
@@ -2526,7 +2578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="3:20">
+    <row r="38" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C38">
         <v>38</v>
       </c>
@@ -2576,7 +2628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="3:20">
+    <row r="39" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C39">
         <v>39</v>
       </c>
@@ -2626,7 +2678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="3:20">
+    <row r="40" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C40">
         <v>40</v>
       </c>
@@ -2676,7 +2728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="3:20">
+    <row r="41" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C41">
         <v>41</v>
       </c>
@@ -2726,7 +2778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="3:20">
+    <row r="42" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C42">
         <v>42</v>
       </c>
@@ -2776,7 +2828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="3:20">
+    <row r="43" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C43">
         <v>43</v>
       </c>
@@ -2826,7 +2878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="3:20">
+    <row r="44" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C44">
         <v>44</v>
       </c>
@@ -2876,7 +2928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="3:20">
+    <row r="45" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C45">
         <v>45</v>
       </c>
@@ -2926,7 +2978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="3:20">
+    <row r="46" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C46">
         <v>46</v>
       </c>
@@ -2976,7 +3028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="3:20">
+    <row r="47" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C47">
         <v>47</v>
       </c>
@@ -3026,7 +3078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="3:20">
+    <row r="48" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C48">
         <v>48</v>
       </c>
@@ -3076,7 +3128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:24">
+    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>25</v>
       </c>
@@ -3138,7 +3190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:24">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C50">
         <v>50</v>
       </c>
@@ -3191,7 +3243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:24">
+    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C51">
         <v>51</v>
       </c>
@@ -3244,7 +3296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:24">
+    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C52">
         <v>52</v>
       </c>
@@ -3258,7 +3310,7 @@
         <v>0</v>
       </c>
       <c r="G52">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H52">
         <v>0</v>
@@ -3288,7 +3340,7 @@
         <v>0</v>
       </c>
       <c r="Q52">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U52">
         <v>0</v>
@@ -3297,7 +3349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:24">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C53">
         <v>53</v>
       </c>
@@ -3311,7 +3363,7 @@
         <v>0</v>
       </c>
       <c r="G53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H53">
         <v>0</v>
@@ -3341,7 +3393,7 @@
         <v>0</v>
       </c>
       <c r="Q53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U53">
         <v>0</v>
@@ -3350,7 +3402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:24">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C54">
         <v>54</v>
       </c>
@@ -3364,7 +3416,7 @@
         <v>0</v>
       </c>
       <c r="G54">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H54">
         <v>0</v>
@@ -3394,13 +3446,13 @@
         <v>0</v>
       </c>
       <c r="Q54">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U54">
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:24">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>31</v>
       </c>
@@ -3417,7 +3469,7 @@
         <v>0</v>
       </c>
       <c r="G55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H55">
         <v>0</v>
@@ -3447,7 +3499,7 @@
         <v>0</v>
       </c>
       <c r="Q55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V55">
         <v>0</v>
@@ -3459,7 +3511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:24">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C56">
         <v>56</v>
       </c>
@@ -3473,7 +3525,7 @@
         <v>0</v>
       </c>
       <c r="G56">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H56">
         <v>0</v>
@@ -3503,7 +3555,7 @@
         <v>0</v>
       </c>
       <c r="Q56">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="V56">
         <v>0</v>
@@ -3512,7 +3564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:24">
+    <row r="57" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C57">
         <v>57</v>
       </c>
@@ -3565,7 +3617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:24">
+    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C58">
         <v>58</v>
       </c>
@@ -3618,7 +3670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:24">
+    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C59">
         <v>59</v>
       </c>
@@ -3632,7 +3684,7 @@
         <v>0</v>
       </c>
       <c r="G59">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H59">
         <v>0</v>
@@ -3662,7 +3714,7 @@
         <v>0</v>
       </c>
       <c r="Q59">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V59">
         <v>0</v>
@@ -3671,7 +3723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:24">
+    <row r="60" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C60">
         <v>60</v>
       </c>
@@ -3724,7 +3776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:24">
+    <row r="61" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C61">
         <v>61</v>
       </c>
@@ -3738,7 +3790,7 @@
         <v>0</v>
       </c>
       <c r="G61">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H61">
         <v>0</v>
@@ -3768,7 +3820,7 @@
         <v>0</v>
       </c>
       <c r="Q61">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="V61">
         <v>0</v>
@@ -3777,7 +3829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:24">
+    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C62">
         <v>62</v>
       </c>
@@ -3830,7 +3882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:24">
+    <row r="63" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C63">
         <v>63</v>
       </c>
@@ -3883,7 +3935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:24">
+    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C64">
         <v>64</v>
       </c>
@@ -3936,7 +3988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:23">
+    <row r="65" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C65">
         <v>65</v>
       </c>
@@ -3989,7 +4041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:23">
+    <row r="66" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C66">
         <v>66</v>
       </c>
@@ -4003,7 +4055,7 @@
         <v>0</v>
       </c>
       <c r="G66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H66">
         <v>0</v>
@@ -4033,7 +4085,7 @@
         <v>0</v>
       </c>
       <c r="Q66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V66">
         <v>0</v>
@@ -4042,7 +4094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:23">
+    <row r="67" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C67">
         <v>67</v>
       </c>
@@ -4095,7 +4147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:23">
+    <row r="68" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C68">
         <v>68</v>
       </c>
@@ -4148,7 +4200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:23">
+    <row r="69" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C69">
         <v>69</v>
       </c>
@@ -4201,7 +4253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:23">
+    <row r="70" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C70">
         <v>70</v>
       </c>
@@ -4254,7 +4306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:23">
+    <row r="71" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C71">
         <v>71</v>
       </c>
@@ -4268,7 +4320,7 @@
         <v>0</v>
       </c>
       <c r="G71">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H71">
         <v>0</v>
@@ -4298,7 +4350,7 @@
         <v>0</v>
       </c>
       <c r="Q71">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V71">
         <v>0</v>
@@ -4307,7 +4359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:23">
+    <row r="72" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C72">
         <v>72</v>
       </c>
@@ -4321,7 +4373,7 @@
         <v>0</v>
       </c>
       <c r="G72">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="H72">
         <v>0</v>
@@ -4351,7 +4403,7 @@
         <v>0</v>
       </c>
       <c r="Q72">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="V72">
         <v>0</v>
@@ -4360,7 +4412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:23">
+    <row r="73" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C73">
         <v>73</v>
       </c>
@@ -4374,7 +4426,7 @@
         <v>0</v>
       </c>
       <c r="G73">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="H73">
         <v>0</v>
@@ -4404,7 +4456,7 @@
         <v>0</v>
       </c>
       <c r="Q73">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="V73">
         <v>0</v>
@@ -4413,7 +4465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:23">
+    <row r="74" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C74">
         <v>74</v>
       </c>
@@ -4427,7 +4479,7 @@
         <v>0</v>
       </c>
       <c r="G74">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="H74">
         <v>0</v>
@@ -4457,13 +4509,13 @@
         <v>0</v>
       </c>
       <c r="Q74">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="V74">
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:23">
+    <row r="75" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
all files: Filter out all clients < 18 yo and specify megareport file location
</commit_message>
<xml_diff>
--- a/crisis_src/crisis_sfy_2021.xlsx
+++ b/crisis_src/crisis_sfy_2021.xlsx
@@ -8,25 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KHIT docs\KHIT-scripts\crisis_src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1316D034-D6DE-4450-AECE-BE0FC790A6FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{003EBB51-988F-4B67-9A98-8A2AF19ECEAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21585" windowHeight="11805" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21585" windowHeight="11805" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="crisis_src" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -309,7 +298,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -324,12 +313,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -367,13 +350,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -715,7 +696,7 @@
   <dimension ref="A1:X75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,7 +839,7 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>217</v>
+        <v>0</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -888,7 +869,7 @@
         <v>0</v>
       </c>
       <c r="Q3">
-        <v>217</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
@@ -905,7 +886,7 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -935,7 +916,7 @@
         <v>0</v>
       </c>
       <c r="Q4">
-        <v>29</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
@@ -952,7 +933,7 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <v>246</v>
+        <v>0</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -982,7 +963,7 @@
         <v>0</v>
       </c>
       <c r="Q5">
-        <v>246</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
@@ -1031,10 +1012,6 @@
       <c r="Q6">
         <v>0</v>
       </c>
-      <c r="R6">
-        <f>Q6/Q3</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C7">
@@ -1082,10 +1059,6 @@
       <c r="Q7">
         <v>0</v>
       </c>
-      <c r="R7">
-        <f>Q7/Q3</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C8">
@@ -1133,10 +1106,6 @@
       <c r="Q8">
         <v>0</v>
       </c>
-      <c r="R8">
-        <f>Q8/Q3</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C9">
@@ -1184,10 +1153,6 @@
       <c r="Q9">
         <v>0</v>
       </c>
-      <c r="R9">
-        <f>Q9/Q3</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C10">
@@ -1235,10 +1200,6 @@
       <c r="Q10">
         <v>0</v>
       </c>
-      <c r="R10">
-        <f>Q10/Q3</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C11">
@@ -1286,10 +1247,6 @@
       <c r="Q11">
         <v>0</v>
       </c>
-      <c r="R11">
-        <f>Q11/Q3</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C12">
@@ -1337,10 +1294,6 @@
       <c r="Q12">
         <v>0</v>
       </c>
-      <c r="R12">
-        <f>Q12/Q3</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C13">
@@ -1388,10 +1341,6 @@
       <c r="Q13">
         <v>0</v>
       </c>
-      <c r="R13">
-        <f>Q13/Q3</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C14">
@@ -1439,10 +1388,6 @@
       <c r="Q14">
         <v>0</v>
       </c>
-      <c r="R14">
-        <f>Q14/Q3</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C15">
@@ -1490,10 +1435,6 @@
       <c r="Q15">
         <v>0</v>
       </c>
-      <c r="R15">
-        <f>Q15/Q3</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C16">
@@ -1541,12 +1482,8 @@
       <c r="Q16">
         <v>0</v>
       </c>
-      <c r="R16">
-        <f>Q16/Q3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C17">
         <v>17</v>
       </c>
@@ -1560,7 +1497,7 @@
         <v>0</v>
       </c>
       <c r="G17">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="H17">
         <v>0</v>
@@ -1590,14 +1527,10 @@
         <v>0</v>
       </c>
       <c r="Q17">
-        <v>60</v>
-      </c>
-      <c r="R17">
-        <f>Q17/Q3</f>
-        <v>0.27649769585253459</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>28</v>
       </c>
@@ -1614,7 +1547,7 @@
         <v>0</v>
       </c>
       <c r="G18">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="H18">
         <v>0</v>
@@ -1644,18 +1577,10 @@
         <v>0</v>
       </c>
       <c r="Q18">
-        <v>19</v>
-      </c>
-      <c r="R18">
-        <f>Q18/Q3</f>
-        <v>8.755760368663594E-2</v>
-      </c>
-      <c r="S18">
-        <f>(Q18+Q19+Q20)/Q3</f>
-        <v>0.12442396313364056</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C19">
         <v>19</v>
       </c>
@@ -1669,7 +1594,7 @@
         <v>0</v>
       </c>
       <c r="G19">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -1699,14 +1624,10 @@
         <v>0</v>
       </c>
       <c r="Q19">
-        <v>3</v>
-      </c>
-      <c r="R19">
-        <f>Q19/Q3</f>
-        <v>1.3824884792626729E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C20">
         <v>20</v>
       </c>
@@ -1720,7 +1641,7 @@
         <v>0</v>
       </c>
       <c r="G20">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -1750,14 +1671,10 @@
         <v>0</v>
       </c>
       <c r="Q20">
-        <v>5</v>
-      </c>
-      <c r="R20">
-        <f>Q20/Q3</f>
-        <v>2.3041474654377881E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>29</v>
       </c>
@@ -1774,7 +1691,7 @@
         <v>0</v>
       </c>
       <c r="G21">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="H21">
         <v>0</v>
@@ -1804,14 +1721,10 @@
         <v>0</v>
       </c>
       <c r="Q21">
-        <v>23</v>
-      </c>
-      <c r="R21">
-        <f>Q21/Q3</f>
-        <v>0.10599078341013825</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C22">
         <v>22</v>
       </c>
@@ -1857,12 +1770,8 @@
       <c r="Q22">
         <v>0</v>
       </c>
-      <c r="R22">
-        <f>Q22/Q3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>23</v>
       </c>
@@ -1908,12 +1817,8 @@
       <c r="Q23">
         <v>0</v>
       </c>
-      <c r="R23">
-        <f>Q23/Q3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C24">
         <v>24</v>
       </c>
@@ -1959,12 +1864,8 @@
       <c r="Q24">
         <v>0</v>
       </c>
-      <c r="R24">
-        <f>Q24/Q3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C25">
         <v>25</v>
       </c>
@@ -2010,12 +1911,8 @@
       <c r="Q25">
         <v>0</v>
       </c>
-      <c r="R25">
-        <f>Q25/Q3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C26">
         <v>26</v>
       </c>
@@ -2061,12 +1958,8 @@
       <c r="Q26">
         <v>0</v>
       </c>
-      <c r="R26">
-        <f>Q26/Q3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C27">
         <v>27</v>
       </c>
@@ -2080,7 +1973,7 @@
         <v>0</v>
       </c>
       <c r="G27">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="H27">
         <v>0</v>
@@ -2112,12 +2005,8 @@
       <c r="Q27">
         <v>0</v>
       </c>
-      <c r="R27">
-        <f>Q27/Q3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C28">
         <v>28</v>
       </c>
@@ -2163,12 +2052,8 @@
       <c r="Q28">
         <v>0</v>
       </c>
-      <c r="R28">
-        <f>Q28/Q3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C29">
         <v>29</v>
       </c>
@@ -2214,12 +2099,8 @@
       <c r="Q29">
         <v>0</v>
       </c>
-      <c r="R29">
-        <f>Q29/Q3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>24</v>
       </c>
@@ -2268,12 +2149,8 @@
       <c r="Q30">
         <v>0</v>
       </c>
-      <c r="T30">
-        <f>Q30/Q3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C31">
         <v>31</v>
       </c>
@@ -2287,7 +2164,7 @@
         <v>0</v>
       </c>
       <c r="G31">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H31">
         <v>0</v>
@@ -2317,14 +2194,10 @@
         <v>0</v>
       </c>
       <c r="Q31">
-        <v>10</v>
-      </c>
-      <c r="T31">
-        <f>Q31/Q3</f>
-        <v>4.6082949308755762E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C32">
         <v>32</v>
       </c>
@@ -2338,7 +2211,7 @@
         <v>0</v>
       </c>
       <c r="G32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H32">
         <v>0</v>
@@ -2368,14 +2241,10 @@
         <v>0</v>
       </c>
       <c r="Q32">
-        <v>1</v>
-      </c>
-      <c r="T32">
-        <f>Q32/Q3</f>
-        <v>4.608294930875576E-3</v>
-      </c>
-    </row>
-    <row r="33" spans="3:20" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C33">
         <v>33</v>
       </c>
@@ -2421,12 +2290,8 @@
       <c r="Q33">
         <v>0</v>
       </c>
-      <c r="T33">
-        <f>Q33/Q3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="3:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C34">
         <v>34</v>
       </c>
@@ -2472,12 +2337,8 @@
       <c r="Q34">
         <v>0</v>
       </c>
-      <c r="T34">
-        <f>Q34/Q3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="3:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C35">
         <v>35</v>
       </c>
@@ -2523,12 +2384,8 @@
       <c r="Q35">
         <v>0</v>
       </c>
-      <c r="T35">
-        <f>Q35/Q3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="3:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C36">
         <v>36</v>
       </c>
@@ -2542,7 +2399,7 @@
         <v>0</v>
       </c>
       <c r="G36">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H36">
         <v>0</v>
@@ -2572,14 +2429,10 @@
         <v>0</v>
       </c>
       <c r="Q36">
-        <v>6</v>
-      </c>
-      <c r="T36">
-        <f>Q36/Q3</f>
-        <v>2.7649769585253458E-2</v>
-      </c>
-    </row>
-    <row r="37" spans="3:20" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C37">
         <v>37</v>
       </c>
@@ -2625,12 +2478,8 @@
       <c r="Q37">
         <v>0</v>
       </c>
-      <c r="T37">
-        <f>Q37/Q3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="3:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C38">
         <v>38</v>
       </c>
@@ -2644,7 +2493,7 @@
         <v>0</v>
       </c>
       <c r="G38">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H38">
         <v>0</v>
@@ -2674,14 +2523,10 @@
         <v>0</v>
       </c>
       <c r="Q38">
-        <v>2</v>
-      </c>
-      <c r="T38">
-        <f>Q38/Q3</f>
-        <v>9.2165898617511521E-3</v>
-      </c>
-    </row>
-    <row r="39" spans="3:20" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C39">
         <v>39</v>
       </c>
@@ -2727,12 +2572,8 @@
       <c r="Q39">
         <v>0</v>
       </c>
-      <c r="T39">
-        <f>Q39/Q3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="3:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C40">
         <v>40</v>
       </c>
@@ -2778,12 +2619,8 @@
       <c r="Q40">
         <v>0</v>
       </c>
-      <c r="T40">
-        <f>Q40/Q3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="3:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C41">
         <v>41</v>
       </c>
@@ -2797,7 +2634,7 @@
         <v>0</v>
       </c>
       <c r="G41">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H41">
         <v>0</v>
@@ -2827,14 +2664,10 @@
         <v>0</v>
       </c>
       <c r="Q41">
-        <v>6</v>
-      </c>
-      <c r="T41">
-        <f>Q41/Q3</f>
-        <v>2.7649769585253458E-2</v>
-      </c>
-    </row>
-    <row r="42" spans="3:20" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C42">
         <v>42</v>
       </c>
@@ -2880,12 +2713,8 @@
       <c r="Q42">
         <v>0</v>
       </c>
-      <c r="T42">
-        <f>Q42/Q3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="3:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C43">
         <v>43</v>
       </c>
@@ -2931,12 +2760,8 @@
       <c r="Q43">
         <v>0</v>
       </c>
-      <c r="T43">
-        <f>Q43/Q3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="3:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C44">
         <v>44</v>
       </c>
@@ -2982,12 +2807,8 @@
       <c r="Q44">
         <v>0</v>
       </c>
-      <c r="T44">
-        <f>Q44/Q3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="3:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C45">
         <v>45</v>
       </c>
@@ -3033,12 +2854,8 @@
       <c r="Q45">
         <v>0</v>
       </c>
-      <c r="T45">
-        <f>Q45/Q3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="3:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C46">
         <v>46</v>
       </c>
@@ -3084,12 +2901,8 @@
       <c r="Q46">
         <v>0</v>
       </c>
-      <c r="T46">
-        <f>Q46/Q3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="3:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C47">
         <v>47</v>
       </c>
@@ -3103,7 +2916,7 @@
         <v>0</v>
       </c>
       <c r="G47">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H47">
         <v>0</v>
@@ -3133,14 +2946,10 @@
         <v>0</v>
       </c>
       <c r="Q47">
-        <v>4</v>
-      </c>
-      <c r="T47">
-        <f>Q47/Q3</f>
-        <v>1.8433179723502304E-2</v>
-      </c>
-    </row>
-    <row r="48" spans="3:20" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C48">
         <v>48</v>
       </c>
@@ -3186,12 +2995,8 @@
       <c r="Q48">
         <v>0</v>
       </c>
-      <c r="T48">
-        <f>Q48/Q3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>25</v>
       </c>
@@ -3243,20 +3048,8 @@
       <c r="Q49">
         <v>0</v>
       </c>
-      <c r="U49">
-        <f>Q49/Q54</f>
-        <v>0</v>
-      </c>
-      <c r="W49">
-        <f>Q49/Q3</f>
-        <v>0</v>
-      </c>
-      <c r="X49">
-        <f>Q54/Q3</f>
-        <v>1.3824884792626729E-2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C50">
         <v>50</v>
       </c>
@@ -3302,16 +3095,8 @@
       <c r="Q50">
         <v>0</v>
       </c>
-      <c r="U50">
-        <f>Q50/Q54</f>
-        <v>0</v>
-      </c>
-      <c r="W50">
-        <f>Q50/Q3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C51">
         <v>51</v>
       </c>
@@ -3357,16 +3142,8 @@
       <c r="Q51">
         <v>0</v>
       </c>
-      <c r="U51">
-        <f>Q51/Q54</f>
-        <v>0</v>
-      </c>
-      <c r="W51">
-        <f>Q51/Q3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C52">
         <v>52</v>
       </c>
@@ -3380,7 +3157,7 @@
         <v>0</v>
       </c>
       <c r="G52">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H52">
         <v>0</v>
@@ -3410,18 +3187,10 @@
         <v>0</v>
       </c>
       <c r="Q52">
-        <v>2</v>
-      </c>
-      <c r="U52">
-        <f>Q52/Q54</f>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="W52">
-        <f>Q52/Q3</f>
-        <v>9.2165898617511521E-3</v>
-      </c>
-    </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C53">
         <v>53</v>
       </c>
@@ -3435,7 +3204,7 @@
         <v>0</v>
       </c>
       <c r="G53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H53">
         <v>0</v>
@@ -3465,18 +3234,10 @@
         <v>0</v>
       </c>
       <c r="Q53">
-        <v>1</v>
-      </c>
-      <c r="U53">
-        <f>Q53/Q54</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="W53">
-        <f>Q53/Q3</f>
-        <v>4.608294930875576E-3</v>
-      </c>
-    </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C54">
         <v>54</v>
       </c>
@@ -3490,7 +3251,7 @@
         <v>0</v>
       </c>
       <c r="G54">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H54">
         <v>0</v>
@@ -3520,14 +3281,10 @@
         <v>0</v>
       </c>
       <c r="Q54">
-        <v>3</v>
-      </c>
-      <c r="U54">
-        <f>SUM(U49:U53)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>31</v>
       </c>
@@ -3544,7 +3301,7 @@
         <v>0</v>
       </c>
       <c r="G55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H55">
         <v>0</v>
@@ -3574,22 +3331,10 @@
         <v>0</v>
       </c>
       <c r="Q55">
-        <v>1</v>
-      </c>
-      <c r="V55" s="3">
-        <f>Q55/$Q$74</f>
-        <v>1.6666666666666666E-2</v>
-      </c>
-      <c r="W55" s="3">
-        <f>Q55/$Q$3</f>
-        <v>4.608294930875576E-3</v>
-      </c>
-      <c r="X55">
-        <f>Q74/Q3</f>
-        <v>0.27649769585253459</v>
-      </c>
-    </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C56">
         <v>56</v>
       </c>
@@ -3603,7 +3348,7 @@
         <v>0</v>
       </c>
       <c r="G56">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H56">
         <v>0</v>
@@ -3633,18 +3378,10 @@
         <v>0</v>
       </c>
       <c r="Q56">
-        <v>4</v>
-      </c>
-      <c r="V56">
-        <f>Q56/$Q$74</f>
-        <v>6.6666666666666666E-2</v>
-      </c>
-      <c r="W56">
-        <f>Q56/Q3</f>
-        <v>1.8433179723502304E-2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C57">
         <v>57</v>
       </c>
@@ -3690,16 +3427,8 @@
       <c r="Q57">
         <v>0</v>
       </c>
-      <c r="V57">
-        <f>Q57/$Q$74</f>
-        <v>0</v>
-      </c>
-      <c r="W57">
-        <f>Q57/Q3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C58">
         <v>58</v>
       </c>
@@ -3745,16 +3474,8 @@
       <c r="Q58">
         <v>0</v>
       </c>
-      <c r="V58">
-        <f>Q58/$Q$74</f>
-        <v>0</v>
-      </c>
-      <c r="W58">
-        <f>Q58/Q3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C59">
         <v>59</v>
       </c>
@@ -3768,7 +3489,7 @@
         <v>0</v>
       </c>
       <c r="G59">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H59">
         <v>0</v>
@@ -3798,18 +3519,10 @@
         <v>0</v>
       </c>
       <c r="Q59">
-        <v>2</v>
-      </c>
-      <c r="V59">
-        <f>Q59/$Q$74</f>
-        <v>3.3333333333333333E-2</v>
-      </c>
-      <c r="W59">
-        <f>Q59/Q3</f>
-        <v>9.2165898617511521E-3</v>
-      </c>
-    </row>
-    <row r="60" spans="1:24" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C60">
         <v>60</v>
       </c>
@@ -3855,16 +3568,8 @@
       <c r="Q60">
         <v>0</v>
       </c>
-      <c r="V60">
-        <f>Q60/$Q$74</f>
-        <v>0</v>
-      </c>
-      <c r="W60">
-        <f>Q60/Q3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C61">
         <v>61</v>
       </c>
@@ -3878,7 +3583,7 @@
         <v>0</v>
       </c>
       <c r="G61">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H61">
         <v>0</v>
@@ -3908,18 +3613,10 @@
         <v>0</v>
       </c>
       <c r="Q61">
-        <v>5</v>
-      </c>
-      <c r="V61">
-        <f>Q61/Q74</f>
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="W61">
-        <f>Q61/Q3</f>
-        <v>2.3041474654377881E-2</v>
-      </c>
-    </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C62">
         <v>62</v>
       </c>
@@ -3965,16 +3662,8 @@
       <c r="Q62">
         <v>0</v>
       </c>
-      <c r="V62">
-        <f>Q62/Q74</f>
-        <v>0</v>
-      </c>
-      <c r="W62">
-        <f>Q62/Q3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C63">
         <v>63</v>
       </c>
@@ -4020,16 +3709,8 @@
       <c r="Q63">
         <v>0</v>
       </c>
-      <c r="V63">
-        <f>Q63/Q74</f>
-        <v>0</v>
-      </c>
-      <c r="W63">
-        <f>Q63/Q3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C64">
         <v>64</v>
       </c>
@@ -4075,16 +3756,8 @@
       <c r="Q64">
         <v>0</v>
       </c>
-      <c r="V64">
-        <f>Q64/Q74</f>
-        <v>0</v>
-      </c>
-      <c r="W64">
-        <f>Q64/Q3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C65">
         <v>65</v>
       </c>
@@ -4130,16 +3803,8 @@
       <c r="Q65">
         <v>0</v>
       </c>
-      <c r="V65">
-        <f>Q65/Q74</f>
-        <v>0</v>
-      </c>
-      <c r="W65">
-        <f>Q65/Q3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C66">
         <v>66</v>
       </c>
@@ -4153,7 +3818,7 @@
         <v>0</v>
       </c>
       <c r="G66">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H66">
         <v>0</v>
@@ -4183,18 +3848,10 @@
         <v>0</v>
       </c>
       <c r="Q66">
-        <v>1</v>
-      </c>
-      <c r="V66">
-        <f>Q66/Q74</f>
-        <v>1.6666666666666666E-2</v>
-      </c>
-      <c r="W66">
-        <f>Q66/Q3</f>
-        <v>4.608294930875576E-3</v>
-      </c>
-    </row>
-    <row r="67" spans="1:23" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C67">
         <v>67</v>
       </c>
@@ -4240,16 +3897,8 @@
       <c r="Q67">
         <v>0</v>
       </c>
-      <c r="V67">
-        <f>Q67/Q74</f>
-        <v>0</v>
-      </c>
-      <c r="W67">
-        <f>Q67/Q3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C68">
         <v>68</v>
       </c>
@@ -4295,16 +3944,8 @@
       <c r="Q68">
         <v>0</v>
       </c>
-      <c r="V68">
-        <f>Q68/Q74</f>
-        <v>0</v>
-      </c>
-      <c r="W68">
-        <f>Q68/Q3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C69">
         <v>69</v>
       </c>
@@ -4350,16 +3991,8 @@
       <c r="Q69">
         <v>0</v>
       </c>
-      <c r="V69">
-        <f>Q69/Q74</f>
-        <v>0</v>
-      </c>
-      <c r="W69">
-        <f>Q69/Q3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C70">
         <v>70</v>
       </c>
@@ -4405,16 +4038,8 @@
       <c r="Q70">
         <v>0</v>
       </c>
-      <c r="V70">
-        <f>Q70/Q74</f>
-        <v>0</v>
-      </c>
-      <c r="W70">
-        <f>Q70/Q3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C71">
         <v>71</v>
       </c>
@@ -4428,7 +4053,7 @@
         <v>0</v>
       </c>
       <c r="G71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H71">
         <v>0</v>
@@ -4458,18 +4083,10 @@
         <v>0</v>
       </c>
       <c r="Q71">
-        <v>1</v>
-      </c>
-      <c r="V71">
-        <f>Q71/Q74</f>
-        <v>1.6666666666666666E-2</v>
-      </c>
-      <c r="W71">
-        <f>Q71/Q3</f>
-        <v>4.608294930875576E-3</v>
-      </c>
-    </row>
-    <row r="72" spans="1:23" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C72">
         <v>72</v>
       </c>
@@ -4483,7 +4100,7 @@
         <v>0</v>
       </c>
       <c r="G72">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="H72">
         <v>0</v>
@@ -4513,18 +4130,10 @@
         <v>0</v>
       </c>
       <c r="Q72">
-        <v>21</v>
-      </c>
-      <c r="V72">
-        <f>Q72/Q74</f>
-        <v>0.35</v>
-      </c>
-      <c r="W72">
-        <f>Q72/Q3</f>
-        <v>9.6774193548387094E-2</v>
-      </c>
-    </row>
-    <row r="73" spans="1:23" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C73">
         <v>73</v>
       </c>
@@ -4538,7 +4147,7 @@
         <v>0</v>
       </c>
       <c r="G73">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="H73">
         <v>0</v>
@@ -4568,18 +4177,10 @@
         <v>0</v>
       </c>
       <c r="Q73">
-        <v>25</v>
-      </c>
-      <c r="V73">
-        <f>Q73/Q74</f>
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="W73">
-        <f>Q73/Q3</f>
-        <v>0.1152073732718894</v>
-      </c>
-    </row>
-    <row r="74" spans="1:23" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C74">
         <v>74</v>
       </c>
@@ -4593,7 +4194,7 @@
         <v>0</v>
       </c>
       <c r="G74">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="H74">
         <v>0</v>
@@ -4623,14 +4224,10 @@
         <v>0</v>
       </c>
       <c r="Q74">
-        <v>60</v>
-      </c>
-      <c r="V74" s="2">
-        <f>SUM(V55:V73)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:23" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>26</v>
       </c>
@@ -4685,6 +4282,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Create r6-14 and r22-26, mark both as complete
</commit_message>
<xml_diff>
--- a/crisis_src/crisis_sfy_2021.xlsx
+++ b/crisis_src/crisis_sfy_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KHIT docs\KHIT-scripts\crisis_src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{003EBB51-988F-4B67-9A98-8A2AF19ECEAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A513600-7E74-446F-A9B5-543F7E50C87D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21585" windowHeight="11805" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21585" windowHeight="11805" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="crisis_src" sheetId="1" r:id="rId1"/>
@@ -695,8 +695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
r6-14.py: Mark script as complete
</commit_message>
<xml_diff>
--- a/crisis_src/crisis_sfy_2021.xlsx
+++ b/crisis_src/crisis_sfy_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KHIT docs\KHIT-scripts\crisis_src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E27BD4-ED48-421C-97CD-2F7119B9E918}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAEC3DB1-7799-4E13-9AC3-0166C462A01C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="21585" windowHeight="11805" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="crisis_src" sheetId="1" r:id="rId1"/>
@@ -696,7 +696,7 @@
   <dimension ref="A1:X75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1339,7 +1339,7 @@
         <v>0</v>
       </c>
       <c r="Q13">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
@@ -1386,7 +1386,7 @@
         <v>0</v>
       </c>
       <c r="Q14">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
@@ -2050,7 +2050,7 @@
         <v>0</v>
       </c>
       <c r="Q28">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
@@ -2097,7 +2097,7 @@
         <v>0</v>
       </c>
       <c r="Q29">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
claim_details.py: Insert rate_name column and on/off-site summary row
</commit_message>
<xml_diff>
--- a/crisis_src/crisis_sfy_2021.xlsx
+++ b/crisis_src/crisis_sfy_2021.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KHIT docs\KHIT-scripts\crisis_src\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAEC3DB1-7799-4E13-9AC3-0166C462A01C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="crisis_src" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -297,8 +291,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -361,14 +355,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -415,7 +401,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -447,27 +433,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -499,24 +467,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -692,16 +642,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -775,7 +723,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24">
       <c r="C2">
         <v>2</v>
       </c>
@@ -822,7 +770,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24">
       <c r="B3" t="s">
         <v>27</v>
       </c>
@@ -839,7 +787,7 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>327</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -869,10 +817,10 @@
         <v>0</v>
       </c>
       <c r="Q3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24">
       <c r="C4">
         <v>4</v>
       </c>
@@ -886,7 +834,7 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -916,10 +864,10 @@
         <v>0</v>
       </c>
       <c r="Q4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24">
       <c r="C5">
         <v>5</v>
       </c>
@@ -933,7 +881,7 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>381</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -963,10 +911,10 @@
         <v>0</v>
       </c>
       <c r="Q5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24">
       <c r="C6">
         <v>6</v>
       </c>
@@ -1013,7 +961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24">
       <c r="C7">
         <v>7</v>
       </c>
@@ -1060,7 +1008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24">
       <c r="C8">
         <v>8</v>
       </c>
@@ -1074,7 +1022,7 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -1104,10 +1052,10 @@
         <v>0</v>
       </c>
       <c r="Q8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24">
       <c r="C9">
         <v>9</v>
       </c>
@@ -1121,7 +1069,7 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -1151,10 +1099,10 @@
         <v>0</v>
       </c>
       <c r="Q9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24">
       <c r="C10">
         <v>10</v>
       </c>
@@ -1201,7 +1149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24">
       <c r="C11">
         <v>11</v>
       </c>
@@ -1248,7 +1196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24">
       <c r="C12">
         <v>12</v>
       </c>
@@ -1295,7 +1243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24">
       <c r="C13">
         <v>13</v>
       </c>
@@ -1309,7 +1257,7 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -1339,10 +1287,10 @@
         <v>0</v>
       </c>
       <c r="Q13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24">
       <c r="C14">
         <v>14</v>
       </c>
@@ -1356,7 +1304,7 @@
         <v>0</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -1386,10 +1334,10 @@
         <v>0</v>
       </c>
       <c r="Q14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24">
       <c r="C15">
         <v>15</v>
       </c>
@@ -1403,7 +1351,7 @@
         <v>0</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="H15">
         <v>0</v>
@@ -1436,7 +1384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24">
       <c r="C16">
         <v>16</v>
       </c>
@@ -1483,7 +1431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17">
       <c r="C17">
         <v>17</v>
       </c>
@@ -1497,7 +1445,7 @@
         <v>0</v>
       </c>
       <c r="G17">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="H17">
         <v>0</v>
@@ -1527,10 +1475,10 @@
         <v>0</v>
       </c>
       <c r="Q17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
       <c r="B18" t="s">
         <v>28</v>
       </c>
@@ -1547,7 +1495,7 @@
         <v>0</v>
       </c>
       <c r="G18">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="H18">
         <v>0</v>
@@ -1577,10 +1525,10 @@
         <v>0</v>
       </c>
       <c r="Q18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
       <c r="C19">
         <v>19</v>
       </c>
@@ -1594,7 +1542,7 @@
         <v>0</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -1624,10 +1572,10 @@
         <v>0</v>
       </c>
       <c r="Q19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
       <c r="C20">
         <v>20</v>
       </c>
@@ -1641,7 +1589,7 @@
         <v>0</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -1671,10 +1619,10 @@
         <v>0</v>
       </c>
       <c r="Q20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17">
       <c r="B21" t="s">
         <v>29</v>
       </c>
@@ -1691,7 +1639,7 @@
         <v>0</v>
       </c>
       <c r="G21">
-        <v>0</v>
+        <v>101</v>
       </c>
       <c r="H21">
         <v>0</v>
@@ -1721,10 +1669,10 @@
         <v>0</v>
       </c>
       <c r="Q21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17">
       <c r="C22">
         <v>22</v>
       </c>
@@ -1738,7 +1686,7 @@
         <v>0</v>
       </c>
       <c r="G22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H22">
         <v>0</v>
@@ -1768,10 +1716,10 @@
         <v>0</v>
       </c>
       <c r="Q22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17">
       <c r="C23">
         <v>23</v>
       </c>
@@ -1785,7 +1733,7 @@
         <v>0</v>
       </c>
       <c r="G23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H23">
         <v>0</v>
@@ -1815,10 +1763,10 @@
         <v>0</v>
       </c>
       <c r="Q23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17">
       <c r="C24">
         <v>24</v>
       </c>
@@ -1832,7 +1780,7 @@
         <v>0</v>
       </c>
       <c r="G24">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H24">
         <v>0</v>
@@ -1862,10 +1810,10 @@
         <v>0</v>
       </c>
       <c r="Q24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
       <c r="C25">
         <v>25</v>
       </c>
@@ -1879,7 +1827,7 @@
         <v>0</v>
       </c>
       <c r="G25">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="H25">
         <v>0</v>
@@ -1909,10 +1857,10 @@
         <v>0</v>
       </c>
       <c r="Q25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17">
       <c r="C26">
         <v>26</v>
       </c>
@@ -1926,7 +1874,7 @@
         <v>0</v>
       </c>
       <c r="G26">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="H26">
         <v>0</v>
@@ -1956,10 +1904,10 @@
         <v>0</v>
       </c>
       <c r="Q26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17">
       <c r="C27">
         <v>27</v>
       </c>
@@ -1973,7 +1921,7 @@
         <v>0</v>
       </c>
       <c r="G27">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H27">
         <v>0</v>
@@ -2003,10 +1951,10 @@
         <v>0</v>
       </c>
       <c r="Q27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17">
       <c r="C28">
         <v>28</v>
       </c>
@@ -2020,7 +1968,7 @@
         <v>0</v>
       </c>
       <c r="G28">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H28">
         <v>0</v>
@@ -2050,10 +1998,10 @@
         <v>0</v>
       </c>
       <c r="Q28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
       <c r="C29">
         <v>29</v>
       </c>
@@ -2067,7 +2015,7 @@
         <v>0</v>
       </c>
       <c r="G29">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="H29">
         <v>0</v>
@@ -2097,10 +2045,10 @@
         <v>0</v>
       </c>
       <c r="Q29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17">
       <c r="A30" t="s">
         <v>24</v>
       </c>
@@ -2150,7 +2098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17">
       <c r="C31">
         <v>31</v>
       </c>
@@ -2164,7 +2112,7 @@
         <v>0</v>
       </c>
       <c r="G31">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H31">
         <v>0</v>
@@ -2194,10 +2142,10 @@
         <v>0</v>
       </c>
       <c r="Q31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17">
       <c r="C32">
         <v>32</v>
       </c>
@@ -2244,7 +2192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:17">
       <c r="C33">
         <v>33</v>
       </c>
@@ -2291,7 +2239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:17">
       <c r="C34">
         <v>34</v>
       </c>
@@ -2305,7 +2253,7 @@
         <v>0</v>
       </c>
       <c r="G34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H34">
         <v>0</v>
@@ -2335,10 +2283,10 @@
         <v>0</v>
       </c>
       <c r="Q34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="3:17" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="3:17">
       <c r="C35">
         <v>35</v>
       </c>
@@ -2385,7 +2333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:17">
       <c r="C36">
         <v>36</v>
       </c>
@@ -2399,7 +2347,7 @@
         <v>0</v>
       </c>
       <c r="G36">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H36">
         <v>0</v>
@@ -2429,10 +2377,10 @@
         <v>0</v>
       </c>
       <c r="Q36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="3:17" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="3:17">
       <c r="C37">
         <v>37</v>
       </c>
@@ -2479,7 +2427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:17">
       <c r="C38">
         <v>38</v>
       </c>
@@ -2493,7 +2441,7 @@
         <v>0</v>
       </c>
       <c r="G38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H38">
         <v>0</v>
@@ -2523,10 +2471,10 @@
         <v>0</v>
       </c>
       <c r="Q38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="3:17" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="3:17">
       <c r="C39">
         <v>39</v>
       </c>
@@ -2573,7 +2521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:17">
       <c r="C40">
         <v>40</v>
       </c>
@@ -2620,7 +2568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:17">
       <c r="C41">
         <v>41</v>
       </c>
@@ -2667,7 +2615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:17">
       <c r="C42">
         <v>42</v>
       </c>
@@ -2714,7 +2662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:17">
       <c r="C43">
         <v>43</v>
       </c>
@@ -2761,7 +2709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:17">
       <c r="C44">
         <v>44</v>
       </c>
@@ -2808,7 +2756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:17">
       <c r="C45">
         <v>45</v>
       </c>
@@ -2855,7 +2803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:17">
       <c r="C46">
         <v>46</v>
       </c>
@@ -2902,7 +2850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:17">
       <c r="C47">
         <v>47</v>
       </c>
@@ -2916,7 +2864,7 @@
         <v>0</v>
       </c>
       <c r="G47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H47">
         <v>0</v>
@@ -2946,10 +2894,10 @@
         <v>0</v>
       </c>
       <c r="Q47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="3:17" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="3:17">
       <c r="C48">
         <v>48</v>
       </c>
@@ -2996,7 +2944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17">
       <c r="A49" t="s">
         <v>25</v>
       </c>
@@ -3049,7 +2997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17">
       <c r="C50">
         <v>50</v>
       </c>
@@ -3096,7 +3044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17">
       <c r="C51">
         <v>51</v>
       </c>
@@ -3143,7 +3091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17">
       <c r="C52">
         <v>52</v>
       </c>
@@ -3190,7 +3138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17">
       <c r="C53">
         <v>53</v>
       </c>
@@ -3237,7 +3185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17">
       <c r="C54">
         <v>54</v>
       </c>
@@ -3284,7 +3232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17">
       <c r="B55" t="s">
         <v>31</v>
       </c>
@@ -3334,7 +3282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17">
       <c r="C56">
         <v>56</v>
       </c>
@@ -3381,7 +3329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17">
       <c r="C57">
         <v>57</v>
       </c>
@@ -3428,7 +3376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17">
       <c r="C58">
         <v>58</v>
       </c>
@@ -3475,7 +3423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17">
       <c r="C59">
         <v>59</v>
       </c>
@@ -3522,7 +3470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17">
       <c r="C60">
         <v>60</v>
       </c>
@@ -3569,7 +3517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17">
       <c r="C61">
         <v>61</v>
       </c>
@@ -3616,7 +3564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17">
       <c r="C62">
         <v>62</v>
       </c>
@@ -3663,7 +3611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17">
       <c r="C63">
         <v>63</v>
       </c>
@@ -3710,7 +3658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17">
       <c r="C64">
         <v>64</v>
       </c>
@@ -3757,7 +3705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:22">
       <c r="C65">
         <v>65</v>
       </c>
@@ -3804,7 +3752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:22">
       <c r="C66">
         <v>66</v>
       </c>
@@ -3851,7 +3799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:22">
       <c r="C67">
         <v>67</v>
       </c>
@@ -3898,7 +3846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:22">
       <c r="C68">
         <v>68</v>
       </c>
@@ -3945,7 +3893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:22">
       <c r="C69">
         <v>69</v>
       </c>
@@ -3992,7 +3940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:22">
       <c r="C70">
         <v>70</v>
       </c>
@@ -4039,7 +3987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:22">
       <c r="C71">
         <v>71</v>
       </c>
@@ -4086,7 +4034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:22">
       <c r="C72">
         <v>72</v>
       </c>
@@ -4133,7 +4081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:22">
       <c r="C73">
         <v>73</v>
       </c>
@@ -4180,7 +4128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:22">
       <c r="C74">
         <v>74</v>
       </c>
@@ -4227,7 +4175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:22">
       <c r="A75" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
r17: Remove personal algorithm and redo script to use Oaks SQL-based report
</commit_message>
<xml_diff>
--- a/crisis_src/crisis_sfy_2021.xlsx
+++ b/crisis_src/crisis_sfy_2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KHIT docs\KHIT-scripts\crisis_src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E66B1AC0-204E-4B00-A4DC-0F1C2197E30D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A052074-6776-4307-8CB9-02155C4193CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="crisis_src" sheetId="1" r:id="rId1"/>
@@ -696,7 +696,7 @@
   <dimension ref="A1:X75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+      <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1500,7 +1500,7 @@
         <v>0</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="I17">
         <v>0</v>
@@ -1527,7 +1527,7 @@
         <v>0</v>
       </c>
       <c r="Q17">
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
r21: Remove personal algorithm and redo script to use Oaks SQL-based report
</commit_message>
<xml_diff>
--- a/crisis_src/crisis_sfy_2021.xlsx
+++ b/crisis_src/crisis_sfy_2021.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KHIT docs\KHIT-scripts\crisis_src\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A052074-6776-4307-8CB9-02155C4193CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="crisis_src" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -297,8 +291,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -361,14 +355,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -415,7 +401,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -447,27 +433,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -499,24 +467,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -692,16 +642,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -775,7 +723,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24">
       <c r="C2">
         <v>2</v>
       </c>
@@ -822,7 +770,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24">
       <c r="B3" t="s">
         <v>27</v>
       </c>
@@ -872,7 +820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24">
       <c r="C4">
         <v>4</v>
       </c>
@@ -919,7 +867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24">
       <c r="C5">
         <v>5</v>
       </c>
@@ -966,7 +914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24">
       <c r="C6">
         <v>6</v>
       </c>
@@ -1013,7 +961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24">
       <c r="C7">
         <v>7</v>
       </c>
@@ -1060,7 +1008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24">
       <c r="C8">
         <v>8</v>
       </c>
@@ -1107,7 +1055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24">
       <c r="C9">
         <v>9</v>
       </c>
@@ -1154,7 +1102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24">
       <c r="C10">
         <v>10</v>
       </c>
@@ -1201,7 +1149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24">
       <c r="C11">
         <v>11</v>
       </c>
@@ -1248,7 +1196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24">
       <c r="C12">
         <v>12</v>
       </c>
@@ -1295,7 +1243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24">
       <c r="C13">
         <v>13</v>
       </c>
@@ -1342,7 +1290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24">
       <c r="C14">
         <v>14</v>
       </c>
@@ -1389,7 +1337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24">
       <c r="C15">
         <v>15</v>
       </c>
@@ -1436,7 +1384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24">
       <c r="C16">
         <v>16</v>
       </c>
@@ -1483,7 +1431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17">
       <c r="C17">
         <v>17</v>
       </c>
@@ -1530,7 +1478,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17">
       <c r="B18" t="s">
         <v>28</v>
       </c>
@@ -1580,7 +1528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17">
       <c r="C19">
         <v>19</v>
       </c>
@@ -1627,7 +1575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17">
       <c r="C20">
         <v>20</v>
       </c>
@@ -1674,7 +1622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17">
       <c r="B21" t="s">
         <v>29</v>
       </c>
@@ -1694,7 +1642,7 @@
         <v>0</v>
       </c>
       <c r="H21">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="I21">
         <v>0</v>
@@ -1721,10 +1669,10 @@
         <v>0</v>
       </c>
       <c r="Q21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17">
       <c r="C22">
         <v>22</v>
       </c>
@@ -1771,7 +1719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17">
       <c r="C23">
         <v>23</v>
       </c>
@@ -1818,7 +1766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17">
       <c r="C24">
         <v>24</v>
       </c>
@@ -1865,7 +1813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17">
       <c r="C25">
         <v>25</v>
       </c>
@@ -1912,7 +1860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17">
       <c r="C26">
         <v>26</v>
       </c>
@@ -1959,7 +1907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17">
       <c r="C27">
         <v>27</v>
       </c>
@@ -2006,7 +1954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17">
       <c r="C28">
         <v>28</v>
       </c>
@@ -2053,7 +2001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17">
       <c r="C29">
         <v>29</v>
       </c>
@@ -2100,7 +2048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17">
       <c r="A30" t="s">
         <v>24</v>
       </c>
@@ -2150,7 +2098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17">
       <c r="C31">
         <v>31</v>
       </c>
@@ -2197,7 +2145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17">
       <c r="C32">
         <v>32</v>
       </c>
@@ -2244,7 +2192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:17">
       <c r="C33">
         <v>33</v>
       </c>
@@ -2291,7 +2239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:17">
       <c r="C34">
         <v>34</v>
       </c>
@@ -2338,7 +2286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:17">
       <c r="C35">
         <v>35</v>
       </c>
@@ -2385,7 +2333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:17">
       <c r="C36">
         <v>36</v>
       </c>
@@ -2432,7 +2380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:17">
       <c r="C37">
         <v>37</v>
       </c>
@@ -2479,7 +2427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:17">
       <c r="C38">
         <v>38</v>
       </c>
@@ -2526,7 +2474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:17">
       <c r="C39">
         <v>39</v>
       </c>
@@ -2573,7 +2521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:17">
       <c r="C40">
         <v>40</v>
       </c>
@@ -2620,7 +2568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:17">
       <c r="C41">
         <v>41</v>
       </c>
@@ -2667,7 +2615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:17">
       <c r="C42">
         <v>42</v>
       </c>
@@ -2714,7 +2662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:17">
       <c r="C43">
         <v>43</v>
       </c>
@@ -2761,7 +2709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:17">
       <c r="C44">
         <v>44</v>
       </c>
@@ -2808,7 +2756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:17">
       <c r="C45">
         <v>45</v>
       </c>
@@ -2855,7 +2803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:17">
       <c r="C46">
         <v>46</v>
       </c>
@@ -2902,7 +2850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:17">
       <c r="C47">
         <v>47</v>
       </c>
@@ -2949,7 +2897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:17">
       <c r="C48">
         <v>48</v>
       </c>
@@ -2996,7 +2944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17">
       <c r="A49" t="s">
         <v>25</v>
       </c>
@@ -3049,7 +2997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17">
       <c r="C50">
         <v>50</v>
       </c>
@@ -3096,7 +3044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17">
       <c r="C51">
         <v>51</v>
       </c>
@@ -3143,7 +3091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17">
       <c r="C52">
         <v>52</v>
       </c>
@@ -3190,7 +3138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17">
       <c r="C53">
         <v>53</v>
       </c>
@@ -3237,7 +3185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17">
       <c r="C54">
         <v>54</v>
       </c>
@@ -3284,7 +3232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17">
       <c r="B55" t="s">
         <v>31</v>
       </c>
@@ -3334,7 +3282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17">
       <c r="C56">
         <v>56</v>
       </c>
@@ -3381,7 +3329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17">
       <c r="C57">
         <v>57</v>
       </c>
@@ -3428,7 +3376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17">
       <c r="C58">
         <v>58</v>
       </c>
@@ -3475,7 +3423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17">
       <c r="C59">
         <v>59</v>
       </c>
@@ -3522,7 +3470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17">
       <c r="C60">
         <v>60</v>
       </c>
@@ -3569,7 +3517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17">
       <c r="C61">
         <v>61</v>
       </c>
@@ -3616,7 +3564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17">
       <c r="C62">
         <v>62</v>
       </c>
@@ -3663,7 +3611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17">
       <c r="C63">
         <v>63</v>
       </c>
@@ -3710,7 +3658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17">
       <c r="C64">
         <v>64</v>
       </c>
@@ -3757,7 +3705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:22">
       <c r="C65">
         <v>65</v>
       </c>
@@ -3804,7 +3752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:22">
       <c r="C66">
         <v>66</v>
       </c>
@@ -3851,7 +3799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:22">
       <c r="C67">
         <v>67</v>
       </c>
@@ -3898,7 +3846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:22">
       <c r="C68">
         <v>68</v>
       </c>
@@ -3945,7 +3893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:22">
       <c r="C69">
         <v>69</v>
       </c>
@@ -3992,7 +3940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:22">
       <c r="C70">
         <v>70</v>
       </c>
@@ -4039,7 +3987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:22">
       <c r="C71">
         <v>71</v>
       </c>
@@ -4086,7 +4034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:22">
       <c r="C72">
         <v>72</v>
       </c>
@@ -4133,7 +4081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:22">
       <c r="C73">
         <v>73</v>
       </c>
@@ -4180,7 +4128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:22">
       <c r="C74">
         <v>74</v>
       </c>
@@ -4227,7 +4175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:22">
       <c r="A75" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
r27: Remove personal algorithm and redo script to use Oaks SQL-based report
</commit_message>
<xml_diff>
--- a/crisis_src/crisis_sfy_2021.xlsx
+++ b/crisis_src/crisis_sfy_2021.xlsx
@@ -1924,7 +1924,7 @@
         <v>0</v>
       </c>
       <c r="H27">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I27">
         <v>0</v>
@@ -1951,7 +1951,7 @@
         <v>0</v>
       </c>
       <c r="Q27">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:17">

</xml_diff>

<commit_message>
r18_20: Remove personal algorithm and redo script to use Oaks SQL-based report
</commit_message>
<xml_diff>
--- a/crisis_src/crisis_sfy_2021.xlsx
+++ b/crisis_src/crisis_sfy_2021.xlsx
@@ -1498,7 +1498,7 @@
         <v>0</v>
       </c>
       <c r="H18">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="I18">
         <v>0</v>
@@ -1525,7 +1525,7 @@
         <v>0</v>
       </c>
       <c r="Q18">
-        <v>0</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:17">
@@ -1592,7 +1592,7 @@
         <v>0</v>
       </c>
       <c r="H20">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="I20">
         <v>0</v>
@@ -1619,7 +1619,7 @@
         <v>0</v>
       </c>
       <c r="Q20">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:17">

</xml_diff>

<commit_message>
r28_29: Update script to use Oaks' predefined SQL custom report
</commit_message>
<xml_diff>
--- a/crisis_src/crisis_sfy_2021.xlsx
+++ b/crisis_src/crisis_sfy_2021.xlsx
@@ -1971,7 +1971,7 @@
         <v>0</v>
       </c>
       <c r="H28">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I28">
         <v>0</v>
@@ -1998,7 +1998,7 @@
         <v>0</v>
       </c>
       <c r="Q28">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:17">
@@ -2018,7 +2018,7 @@
         <v>0</v>
       </c>
       <c r="H29">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="I29">
         <v>0</v>
@@ -2045,7 +2045,7 @@
         <v>0</v>
       </c>
       <c r="Q29">
-        <v>0</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:17">

</xml_diff>

<commit_message>
r30_48: Update script to use Oaks' predefined SQL custom report
</commit_message>
<xml_diff>
--- a/crisis_src/crisis_sfy_2021.xlsx
+++ b/crisis_src/crisis_sfy_2021.xlsx
@@ -2118,7 +2118,7 @@
         <v>0</v>
       </c>
       <c r="I31">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J31">
         <v>0</v>
@@ -2142,7 +2142,7 @@
         <v>0</v>
       </c>
       <c r="Q31">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:17">
@@ -2212,7 +2212,7 @@
         <v>0</v>
       </c>
       <c r="I33">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J33">
         <v>0</v>
@@ -2236,7 +2236,7 @@
         <v>0</v>
       </c>
       <c r="Q33">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="3:17">
@@ -2259,7 +2259,7 @@
         <v>0</v>
       </c>
       <c r="I34">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="J34">
         <v>0</v>
@@ -2283,7 +2283,7 @@
         <v>0</v>
       </c>
       <c r="Q34">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="35" spans="3:17">
@@ -2353,7 +2353,7 @@
         <v>0</v>
       </c>
       <c r="I36">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="J36">
         <v>0</v>
@@ -2377,7 +2377,7 @@
         <v>0</v>
       </c>
       <c r="Q36">
-        <v>0</v>
+        <v>28</v>
       </c>
     </row>
     <row r="37" spans="3:17">
@@ -2541,7 +2541,7 @@
         <v>0</v>
       </c>
       <c r="I40">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J40">
         <v>0</v>
@@ -2565,7 +2565,7 @@
         <v>0</v>
       </c>
       <c r="Q40">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41" spans="3:17">
@@ -2588,7 +2588,7 @@
         <v>0</v>
       </c>
       <c r="I41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J41">
         <v>0</v>
@@ -2612,7 +2612,7 @@
         <v>0</v>
       </c>
       <c r="Q41">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="3:17">
@@ -2682,7 +2682,7 @@
         <v>0</v>
       </c>
       <c r="I43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J43">
         <v>0</v>
@@ -2706,7 +2706,7 @@
         <v>0</v>
       </c>
       <c r="Q43">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="3:17">
@@ -2823,7 +2823,7 @@
         <v>0</v>
       </c>
       <c r="I46">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J46">
         <v>0</v>
@@ -2847,7 +2847,7 @@
         <v>0</v>
       </c>
       <c r="Q46">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="47" spans="3:17">
@@ -2870,7 +2870,7 @@
         <v>0</v>
       </c>
       <c r="I47">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="J47">
         <v>0</v>
@@ -2894,7 +2894,7 @@
         <v>0</v>
       </c>
       <c r="Q47">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="48" spans="3:17">

</xml_diff>

<commit_message>
Update various files to use previous month date
</commit_message>
<xml_diff>
--- a/crisis_src/crisis_sfy_2021.xlsx
+++ b/crisis_src/crisis_sfy_2021.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KHIT docs\KHIT-scripts\crisis_src\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{296C7F1A-6725-48C0-9460-3D08A6C846D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="crisis_src" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -291,8 +297,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -355,6 +361,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -401,7 +415,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -433,9 +447,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -467,6 +499,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -642,14 +692,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -723,7 +775,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C2">
         <v>2</v>
       </c>
@@ -770,7 +822,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>27</v>
       </c>
@@ -820,7 +872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>4</v>
       </c>
@@ -867,7 +919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>5</v>
       </c>
@@ -914,7 +966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>6</v>
       </c>
@@ -961,7 +1013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>7</v>
       </c>
@@ -1008,7 +1060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>8</v>
       </c>
@@ -1055,7 +1107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>9</v>
       </c>
@@ -1102,7 +1154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C10">
         <v>10</v>
       </c>
@@ -1149,7 +1201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:24">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>11</v>
       </c>
@@ -1196,7 +1248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:24">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C12">
         <v>12</v>
       </c>
@@ -1243,7 +1295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:24">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C13">
         <v>13</v>
       </c>
@@ -1290,7 +1342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:24">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C14">
         <v>14</v>
       </c>
@@ -1337,7 +1389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:24">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C15">
         <v>15</v>
       </c>
@@ -1384,7 +1436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:24">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C16">
         <v>16</v>
       </c>
@@ -1431,7 +1483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C17">
         <v>17</v>
       </c>
@@ -1448,7 +1500,7 @@
         <v>0</v>
       </c>
       <c r="H17">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="I17">
         <v>0</v>
@@ -1475,10 +1527,10 @@
         <v>0</v>
       </c>
       <c r="Q17">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>28</v>
       </c>
@@ -1498,7 +1550,7 @@
         <v>0</v>
       </c>
       <c r="H18">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="I18">
         <v>0</v>
@@ -1525,10 +1577,10 @@
         <v>0</v>
       </c>
       <c r="Q18">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C19">
         <v>19</v>
       </c>
@@ -1575,7 +1627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:17">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C20">
         <v>20</v>
       </c>
@@ -1592,7 +1644,7 @@
         <v>0</v>
       </c>
       <c r="H20">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="I20">
         <v>0</v>
@@ -1619,10 +1671,10 @@
         <v>0</v>
       </c>
       <c r="Q20">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>29</v>
       </c>
@@ -1642,7 +1694,7 @@
         <v>0</v>
       </c>
       <c r="H21">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="I21">
         <v>0</v>
@@ -1669,10 +1721,10 @@
         <v>0</v>
       </c>
       <c r="Q21">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C22">
         <v>22</v>
       </c>
@@ -1719,7 +1771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:17">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>23</v>
       </c>
@@ -1766,7 +1818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:17">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C24">
         <v>24</v>
       </c>
@@ -1813,7 +1865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C25">
         <v>25</v>
       </c>
@@ -1860,7 +1912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:17">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C26">
         <v>26</v>
       </c>
@@ -1907,7 +1959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:17">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C27">
         <v>27</v>
       </c>
@@ -1924,7 +1976,7 @@
         <v>0</v>
       </c>
       <c r="H27">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I27">
         <v>0</v>
@@ -1951,10 +2003,10 @@
         <v>0</v>
       </c>
       <c r="Q27">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C28">
         <v>28</v>
       </c>
@@ -1971,7 +2023,7 @@
         <v>0</v>
       </c>
       <c r="H28">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I28">
         <v>0</v>
@@ -1998,10 +2050,10 @@
         <v>0</v>
       </c>
       <c r="Q28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C29">
         <v>29</v>
       </c>
@@ -2018,7 +2070,7 @@
         <v>0</v>
       </c>
       <c r="H29">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="I29">
         <v>0</v>
@@ -2045,10 +2097,10 @@
         <v>0</v>
       </c>
       <c r="Q29">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>24</v>
       </c>
@@ -2098,7 +2150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:17">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C31">
         <v>31</v>
       </c>
@@ -2118,7 +2170,7 @@
         <v>0</v>
       </c>
       <c r="I31">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J31">
         <v>0</v>
@@ -2142,10 +2194,10 @@
         <v>0</v>
       </c>
       <c r="Q31">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C32">
         <v>32</v>
       </c>
@@ -2192,7 +2244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="3:17">
+    <row r="33" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C33">
         <v>33</v>
       </c>
@@ -2212,7 +2264,7 @@
         <v>0</v>
       </c>
       <c r="I33">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J33">
         <v>0</v>
@@ -2236,10 +2288,10 @@
         <v>0</v>
       </c>
       <c r="Q33">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="3:17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C34">
         <v>34</v>
       </c>
@@ -2259,7 +2311,7 @@
         <v>0</v>
       </c>
       <c r="I34">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="J34">
         <v>0</v>
@@ -2283,10 +2335,10 @@
         <v>0</v>
       </c>
       <c r="Q34">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="35" spans="3:17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C35">
         <v>35</v>
       </c>
@@ -2333,7 +2385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="3:17">
+    <row r="36" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C36">
         <v>36</v>
       </c>
@@ -2353,7 +2405,7 @@
         <v>0</v>
       </c>
       <c r="I36">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="J36">
         <v>0</v>
@@ -2377,10 +2429,10 @@
         <v>0</v>
       </c>
       <c r="Q36">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="37" spans="3:17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C37">
         <v>37</v>
       </c>
@@ -2427,7 +2479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="3:17">
+    <row r="38" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C38">
         <v>38</v>
       </c>
@@ -2474,7 +2526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="3:17">
+    <row r="39" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C39">
         <v>39</v>
       </c>
@@ -2521,7 +2573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="3:17">
+    <row r="40" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C40">
         <v>40</v>
       </c>
@@ -2541,7 +2593,7 @@
         <v>0</v>
       </c>
       <c r="I40">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J40">
         <v>0</v>
@@ -2565,10 +2617,10 @@
         <v>0</v>
       </c>
       <c r="Q40">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="3:17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C41">
         <v>41</v>
       </c>
@@ -2588,7 +2640,7 @@
         <v>0</v>
       </c>
       <c r="I41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J41">
         <v>0</v>
@@ -2612,10 +2664,10 @@
         <v>0</v>
       </c>
       <c r="Q41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="3:17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C42">
         <v>42</v>
       </c>
@@ -2662,7 +2714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="3:17">
+    <row r="43" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C43">
         <v>43</v>
       </c>
@@ -2682,7 +2734,7 @@
         <v>0</v>
       </c>
       <c r="I43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J43">
         <v>0</v>
@@ -2706,10 +2758,10 @@
         <v>0</v>
       </c>
       <c r="Q43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="3:17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C44">
         <v>44</v>
       </c>
@@ -2756,7 +2808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="3:17">
+    <row r="45" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C45">
         <v>45</v>
       </c>
@@ -2803,7 +2855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="3:17">
+    <row r="46" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C46">
         <v>46</v>
       </c>
@@ -2823,7 +2875,7 @@
         <v>0</v>
       </c>
       <c r="I46">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J46">
         <v>0</v>
@@ -2847,10 +2899,10 @@
         <v>0</v>
       </c>
       <c r="Q46">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="47" spans="3:17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C47">
         <v>47</v>
       </c>
@@ -2870,7 +2922,7 @@
         <v>0</v>
       </c>
       <c r="I47">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="J47">
         <v>0</v>
@@ -2894,10 +2946,10 @@
         <v>0</v>
       </c>
       <c r="Q47">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="48" spans="3:17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C48">
         <v>48</v>
       </c>
@@ -2944,7 +2996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:17">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>25</v>
       </c>
@@ -2997,7 +3049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:17">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C50">
         <v>50</v>
       </c>
@@ -3044,7 +3096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:17">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C51">
         <v>51</v>
       </c>
@@ -3091,7 +3143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:17">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C52">
         <v>52</v>
       </c>
@@ -3138,7 +3190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:17">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C53">
         <v>53</v>
       </c>
@@ -3185,7 +3237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:17">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C54">
         <v>54</v>
       </c>
@@ -3232,7 +3284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:17">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>31</v>
       </c>
@@ -3282,7 +3334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:17">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C56">
         <v>56</v>
       </c>
@@ -3329,7 +3381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:17">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C57">
         <v>57</v>
       </c>
@@ -3376,7 +3428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:17">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C58">
         <v>58</v>
       </c>
@@ -3423,7 +3475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:17">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C59">
         <v>59</v>
       </c>
@@ -3470,7 +3522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:17">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C60">
         <v>60</v>
       </c>
@@ -3517,7 +3569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:17">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C61">
         <v>61</v>
       </c>
@@ -3564,7 +3616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:17">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C62">
         <v>62</v>
       </c>
@@ -3611,7 +3663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:17">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C63">
         <v>63</v>
       </c>
@@ -3658,7 +3710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:17">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C64">
         <v>64</v>
       </c>
@@ -3705,7 +3757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:22">
+    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C65">
         <v>65</v>
       </c>
@@ -3752,7 +3804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:22">
+    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C66">
         <v>66</v>
       </c>
@@ -3799,7 +3851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:22">
+    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C67">
         <v>67</v>
       </c>
@@ -3846,7 +3898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:22">
+    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C68">
         <v>68</v>
       </c>
@@ -3893,7 +3945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:22">
+    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C69">
         <v>69</v>
       </c>
@@ -3940,7 +3992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:22">
+    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C70">
         <v>70</v>
       </c>
@@ -3987,7 +4039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:22">
+    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C71">
         <v>71</v>
       </c>
@@ -4034,7 +4086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:22">
+    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C72">
         <v>72</v>
       </c>
@@ -4081,7 +4133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:22">
+    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C73">
         <v>73</v>
       </c>
@@ -4128,7 +4180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:22">
+    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C74">
         <v>74</v>
       </c>
@@ -4175,7 +4227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:22">
+    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
Finish RPA script updates
</commit_message>
<xml_diff>
--- a/crisis_src/crisis_sfy_2021.xlsx
+++ b/crisis_src/crisis_sfy_2021.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KHIT docs\KHIT-scripts\crisis_src\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{296C7F1A-6725-48C0-9460-3D08A6C846D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="crisis_src" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -297,8 +291,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -361,14 +355,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -415,7 +401,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -447,27 +433,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -499,24 +467,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -692,16 +642,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -775,7 +723,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24">
       <c r="C2">
         <v>2</v>
       </c>
@@ -822,7 +770,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24">
       <c r="B3" t="s">
         <v>27</v>
       </c>
@@ -842,7 +790,7 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>228</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -869,10 +817,10 @@
         <v>0</v>
       </c>
       <c r="Q3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24">
       <c r="C4">
         <v>4</v>
       </c>
@@ -889,7 +837,7 @@
         <v>0</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -916,10 +864,10 @@
         <v>0</v>
       </c>
       <c r="Q4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24">
       <c r="C5">
         <v>5</v>
       </c>
@@ -936,7 +884,7 @@
         <v>0</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>270</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -963,10 +911,10 @@
         <v>0</v>
       </c>
       <c r="Q5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24">
       <c r="C6">
         <v>6</v>
       </c>
@@ -983,7 +931,7 @@
         <v>0</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -1010,10 +958,10 @@
         <v>0</v>
       </c>
       <c r="Q6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24">
       <c r="C7">
         <v>7</v>
       </c>
@@ -1030,7 +978,7 @@
         <v>0</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -1057,10 +1005,10 @@
         <v>0</v>
       </c>
       <c r="Q7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24">
       <c r="C8">
         <v>8</v>
       </c>
@@ -1077,7 +1025,7 @@
         <v>0</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>82</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -1104,10 +1052,10 @@
         <v>0</v>
       </c>
       <c r="Q8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24">
       <c r="C9">
         <v>9</v>
       </c>
@@ -1124,7 +1072,7 @@
         <v>0</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -1151,10 +1099,10 @@
         <v>0</v>
       </c>
       <c r="Q9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24">
       <c r="C10">
         <v>10</v>
       </c>
@@ -1171,7 +1119,7 @@
         <v>0</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I10">
         <v>0</v>
@@ -1198,10 +1146,10 @@
         <v>0</v>
       </c>
       <c r="Q10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24">
       <c r="C11">
         <v>11</v>
       </c>
@@ -1248,7 +1196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24">
       <c r="C12">
         <v>12</v>
       </c>
@@ -1295,7 +1243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24">
       <c r="C13">
         <v>13</v>
       </c>
@@ -1312,7 +1260,7 @@
         <v>0</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="I13">
         <v>0</v>
@@ -1339,10 +1287,10 @@
         <v>0</v>
       </c>
       <c r="Q13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24">
       <c r="C14">
         <v>14</v>
       </c>
@@ -1359,7 +1307,7 @@
         <v>0</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>132</v>
       </c>
       <c r="I14">
         <v>0</v>
@@ -1386,10 +1334,10 @@
         <v>0</v>
       </c>
       <c r="Q14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24">
       <c r="C15">
         <v>15</v>
       </c>
@@ -1406,7 +1354,7 @@
         <v>0</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="I15">
         <v>0</v>
@@ -1436,7 +1384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24">
       <c r="C16">
         <v>16</v>
       </c>
@@ -1483,7 +1431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17">
       <c r="C17">
         <v>17</v>
       </c>
@@ -1500,7 +1448,7 @@
         <v>0</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="I17">
         <v>0</v>
@@ -1527,10 +1475,10 @@
         <v>0</v>
       </c>
       <c r="Q17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
       <c r="B18" t="s">
         <v>28</v>
       </c>
@@ -1550,7 +1498,7 @@
         <v>0</v>
       </c>
       <c r="H18">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="I18">
         <v>0</v>
@@ -1577,10 +1525,10 @@
         <v>0</v>
       </c>
       <c r="Q18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
       <c r="C19">
         <v>19</v>
       </c>
@@ -1627,7 +1575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17">
       <c r="C20">
         <v>20</v>
       </c>
@@ -1644,7 +1592,7 @@
         <v>0</v>
       </c>
       <c r="H20">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="I20">
         <v>0</v>
@@ -1671,10 +1619,10 @@
         <v>0</v>
       </c>
       <c r="Q20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17">
       <c r="B21" t="s">
         <v>29</v>
       </c>
@@ -1694,7 +1642,7 @@
         <v>0</v>
       </c>
       <c r="H21">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="I21">
         <v>0</v>
@@ -1721,10 +1669,10 @@
         <v>0</v>
       </c>
       <c r="Q21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17">
       <c r="C22">
         <v>22</v>
       </c>
@@ -1741,7 +1689,7 @@
         <v>0</v>
       </c>
       <c r="H22">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I22">
         <v>0</v>
@@ -1768,10 +1716,10 @@
         <v>0</v>
       </c>
       <c r="Q22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17">
       <c r="C23">
         <v>23</v>
       </c>
@@ -1788,7 +1736,7 @@
         <v>0</v>
       </c>
       <c r="H23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I23">
         <v>0</v>
@@ -1815,10 +1763,10 @@
         <v>0</v>
       </c>
       <c r="Q23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17">
       <c r="C24">
         <v>24</v>
       </c>
@@ -1835,7 +1783,7 @@
         <v>0</v>
       </c>
       <c r="H24">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I24">
         <v>0</v>
@@ -1862,10 +1810,10 @@
         <v>0</v>
       </c>
       <c r="Q24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
       <c r="C25">
         <v>25</v>
       </c>
@@ -1882,7 +1830,7 @@
         <v>0</v>
       </c>
       <c r="H25">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="I25">
         <v>0</v>
@@ -1909,10 +1857,10 @@
         <v>0</v>
       </c>
       <c r="Q25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17">
       <c r="C26">
         <v>26</v>
       </c>
@@ -1929,7 +1877,7 @@
         <v>0</v>
       </c>
       <c r="H26">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="I26">
         <v>0</v>
@@ -1956,10 +1904,10 @@
         <v>0</v>
       </c>
       <c r="Q26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17">
       <c r="C27">
         <v>27</v>
       </c>
@@ -1976,7 +1924,7 @@
         <v>0</v>
       </c>
       <c r="H27">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I27">
         <v>0</v>
@@ -2003,10 +1951,10 @@
         <v>0</v>
       </c>
       <c r="Q27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17">
       <c r="C28">
         <v>28</v>
       </c>
@@ -2023,7 +1971,7 @@
         <v>0</v>
       </c>
       <c r="H28">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I28">
         <v>0</v>
@@ -2050,10 +1998,10 @@
         <v>0</v>
       </c>
       <c r="Q28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
       <c r="C29">
         <v>29</v>
       </c>
@@ -2070,7 +2018,7 @@
         <v>0</v>
       </c>
       <c r="H29">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="I29">
         <v>0</v>
@@ -2097,10 +2045,10 @@
         <v>0</v>
       </c>
       <c r="Q29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17">
       <c r="A30" t="s">
         <v>24</v>
       </c>
@@ -2150,7 +2098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17">
       <c r="C31">
         <v>31</v>
       </c>
@@ -2167,7 +2115,7 @@
         <v>0</v>
       </c>
       <c r="H31">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I31">
         <v>0</v>
@@ -2194,10 +2142,10 @@
         <v>0</v>
       </c>
       <c r="Q31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17">
       <c r="C32">
         <v>32</v>
       </c>
@@ -2244,7 +2192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:17">
       <c r="C33">
         <v>33</v>
       </c>
@@ -2261,7 +2209,7 @@
         <v>0</v>
       </c>
       <c r="H33">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I33">
         <v>0</v>
@@ -2288,10 +2236,10 @@
         <v>0</v>
       </c>
       <c r="Q33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="3:17" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="3:17">
       <c r="C34">
         <v>34</v>
       </c>
@@ -2308,7 +2256,7 @@
         <v>0</v>
       </c>
       <c r="H34">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="I34">
         <v>0</v>
@@ -2335,10 +2283,10 @@
         <v>0</v>
       </c>
       <c r="Q34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="3:17" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="3:17">
       <c r="C35">
         <v>35</v>
       </c>
@@ -2385,7 +2333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:17">
       <c r="C36">
         <v>36</v>
       </c>
@@ -2402,7 +2350,7 @@
         <v>0</v>
       </c>
       <c r="H36">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="I36">
         <v>0</v>
@@ -2429,10 +2377,10 @@
         <v>0</v>
       </c>
       <c r="Q36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="3:17" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="3:17">
       <c r="C37">
         <v>37</v>
       </c>
@@ -2479,7 +2427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:17">
       <c r="C38">
         <v>38</v>
       </c>
@@ -2526,7 +2474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:17">
       <c r="C39">
         <v>39</v>
       </c>
@@ -2573,7 +2521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:17">
       <c r="C40">
         <v>40</v>
       </c>
@@ -2590,7 +2538,7 @@
         <v>0</v>
       </c>
       <c r="H40">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I40">
         <v>0</v>
@@ -2617,10 +2565,10 @@
         <v>0</v>
       </c>
       <c r="Q40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="3:17" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="3:17">
       <c r="C41">
         <v>41</v>
       </c>
@@ -2637,7 +2585,7 @@
         <v>0</v>
       </c>
       <c r="H41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I41">
         <v>0</v>
@@ -2664,10 +2612,10 @@
         <v>0</v>
       </c>
       <c r="Q41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="3:17" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="3:17">
       <c r="C42">
         <v>42</v>
       </c>
@@ -2714,7 +2662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:17">
       <c r="C43">
         <v>43</v>
       </c>
@@ -2731,7 +2679,7 @@
         <v>0</v>
       </c>
       <c r="H43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I43">
         <v>0</v>
@@ -2758,10 +2706,10 @@
         <v>0</v>
       </c>
       <c r="Q43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="3:17" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="3:17">
       <c r="C44">
         <v>44</v>
       </c>
@@ -2808,7 +2756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:17">
       <c r="C45">
         <v>45</v>
       </c>
@@ -2855,7 +2803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:17">
       <c r="C46">
         <v>46</v>
       </c>
@@ -2872,7 +2820,7 @@
         <v>0</v>
       </c>
       <c r="H46">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I46">
         <v>0</v>
@@ -2899,10 +2847,10 @@
         <v>0</v>
       </c>
       <c r="Q46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="3:17" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="3:17">
       <c r="C47">
         <v>47</v>
       </c>
@@ -2919,7 +2867,7 @@
         <v>0</v>
       </c>
       <c r="H47">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I47">
         <v>0</v>
@@ -2946,10 +2894,10 @@
         <v>0</v>
       </c>
       <c r="Q47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="3:17" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="48" spans="3:17">
       <c r="C48">
         <v>48</v>
       </c>
@@ -2996,7 +2944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17">
       <c r="A49" t="s">
         <v>25</v>
       </c>
@@ -3049,7 +2997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17">
       <c r="C50">
         <v>50</v>
       </c>
@@ -3096,7 +3044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17">
       <c r="C51">
         <v>51</v>
       </c>
@@ -3143,7 +3091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17">
       <c r="C52">
         <v>52</v>
       </c>
@@ -3190,7 +3138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17">
       <c r="C53">
         <v>53</v>
       </c>
@@ -3237,7 +3185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17">
       <c r="C54">
         <v>54</v>
       </c>
@@ -3284,7 +3232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17">
       <c r="B55" t="s">
         <v>31</v>
       </c>
@@ -3334,7 +3282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17">
       <c r="C56">
         <v>56</v>
       </c>
@@ -3381,7 +3329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17">
       <c r="C57">
         <v>57</v>
       </c>
@@ -3428,7 +3376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17">
       <c r="C58">
         <v>58</v>
       </c>
@@ -3475,7 +3423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17">
       <c r="C59">
         <v>59</v>
       </c>
@@ -3522,7 +3470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17">
       <c r="C60">
         <v>60</v>
       </c>
@@ -3569,7 +3517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17">
       <c r="C61">
         <v>61</v>
       </c>
@@ -3616,7 +3564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17">
       <c r="C62">
         <v>62</v>
       </c>
@@ -3663,7 +3611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17">
       <c r="C63">
         <v>63</v>
       </c>
@@ -3710,7 +3658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17">
       <c r="C64">
         <v>64</v>
       </c>
@@ -3757,7 +3705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:22">
       <c r="C65">
         <v>65</v>
       </c>
@@ -3804,7 +3752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:22">
       <c r="C66">
         <v>66</v>
       </c>
@@ -3851,7 +3799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:22">
       <c r="C67">
         <v>67</v>
       </c>
@@ -3898,7 +3846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:22">
       <c r="C68">
         <v>68</v>
       </c>
@@ -3945,7 +3893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:22">
       <c r="C69">
         <v>69</v>
       </c>
@@ -3992,7 +3940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:22">
       <c r="C70">
         <v>70</v>
       </c>
@@ -4039,7 +3987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:22">
       <c r="C71">
         <v>71</v>
       </c>
@@ -4086,7 +4034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:22">
       <c r="C72">
         <v>72</v>
       </c>
@@ -4133,7 +4081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:22">
       <c r="C73">
         <v>73</v>
       </c>
@@ -4180,7 +4128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:22">
       <c r="C74">
         <v>74</v>
       </c>
@@ -4227,7 +4175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:22">
       <c r="A75" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
I made a lot of changes... uh paid_claims has been updated I guess lol
</commit_message>
<xml_diff>
--- a/crisis_src/crisis_sfy_2021.xlsx
+++ b/crisis_src/crisis_sfy_2021.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KHIT docs\KHIT-scripts\crisis_src\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C4E611-D6EB-459A-9448-D5121FF8BA4F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="crisis_src" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -291,8 +297,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -308,16 +314,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -340,21 +359,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Calculation" xfId="1" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -401,7 +449,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -433,9 +481,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -467,6 +533,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -642,14 +726,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="10" max="10" width="9.140625" style="3"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -677,7 +766,7 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
@@ -723,7 +812,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C2">
         <v>2</v>
       </c>
@@ -745,7 +834,7 @@
       <c r="I2">
         <v>1</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="3">
         <v>1</v>
       </c>
       <c r="K2">
@@ -770,7 +859,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>27</v>
       </c>
@@ -795,8 +884,8 @@
       <c r="I3">
         <v>0</v>
       </c>
-      <c r="J3">
-        <v>0</v>
+      <c r="J3" s="3">
+        <v>268</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -817,10 +906,10 @@
         <v>0</v>
       </c>
       <c r="Q3">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>4</v>
       </c>
@@ -842,8 +931,8 @@
       <c r="I4">
         <v>0</v>
       </c>
-      <c r="J4">
-        <v>0</v>
+      <c r="J4" s="3">
+        <v>47</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -864,10 +953,10 @@
         <v>0</v>
       </c>
       <c r="Q4">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>5</v>
       </c>
@@ -889,8 +978,8 @@
       <c r="I5">
         <v>0</v>
       </c>
-      <c r="J5">
-        <v>0</v>
+      <c r="J5" s="3">
+        <v>315</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -911,10 +1000,10 @@
         <v>0</v>
       </c>
       <c r="Q5">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>6</v>
       </c>
@@ -936,7 +1025,7 @@
       <c r="I6">
         <v>0</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="3">
         <v>0</v>
       </c>
       <c r="K6">
@@ -961,7 +1050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>7</v>
       </c>
@@ -983,7 +1072,7 @@
       <c r="I7">
         <v>0</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="3">
         <v>0</v>
       </c>
       <c r="K7">
@@ -1008,7 +1097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>8</v>
       </c>
@@ -1030,8 +1119,8 @@
       <c r="I8">
         <v>0</v>
       </c>
-      <c r="J8">
-        <v>0</v>
+      <c r="J8" s="3">
+        <v>52</v>
       </c>
       <c r="K8">
         <v>0</v>
@@ -1052,10 +1141,10 @@
         <v>0</v>
       </c>
       <c r="Q8">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>9</v>
       </c>
@@ -1077,8 +1166,8 @@
       <c r="I9">
         <v>0</v>
       </c>
-      <c r="J9">
-        <v>0</v>
+      <c r="J9" s="3">
+        <v>5</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -1099,10 +1188,10 @@
         <v>0</v>
       </c>
       <c r="Q9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C10">
         <v>10</v>
       </c>
@@ -1124,8 +1213,8 @@
       <c r="I10">
         <v>0</v>
       </c>
-      <c r="J10">
-        <v>0</v>
+      <c r="J10" s="3">
+        <v>7</v>
       </c>
       <c r="K10">
         <v>0</v>
@@ -1146,10 +1235,10 @@
         <v>0</v>
       </c>
       <c r="Q10">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>11</v>
       </c>
@@ -1171,7 +1260,7 @@
       <c r="I11">
         <v>0</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="3">
         <v>0</v>
       </c>
       <c r="K11">
@@ -1196,7 +1285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:24">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C12">
         <v>12</v>
       </c>
@@ -1218,7 +1307,7 @@
       <c r="I12">
         <v>0</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="3">
         <v>0</v>
       </c>
       <c r="K12">
@@ -1243,7 +1332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:24">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C13">
         <v>13</v>
       </c>
@@ -1265,8 +1354,8 @@
       <c r="I13">
         <v>0</v>
       </c>
-      <c r="J13">
-        <v>0</v>
+      <c r="J13" s="3">
+        <v>14</v>
       </c>
       <c r="K13">
         <v>0</v>
@@ -1287,10 +1376,10 @@
         <v>0</v>
       </c>
       <c r="Q13">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C14">
         <v>14</v>
       </c>
@@ -1312,8 +1401,8 @@
       <c r="I14">
         <v>0</v>
       </c>
-      <c r="J14">
-        <v>0</v>
+      <c r="J14" s="3">
+        <v>78</v>
       </c>
       <c r="K14">
         <v>0</v>
@@ -1334,10 +1423,10 @@
         <v>0</v>
       </c>
       <c r="Q14">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C15">
         <v>15</v>
       </c>
@@ -1359,7 +1448,7 @@
       <c r="I15">
         <v>0</v>
       </c>
-      <c r="J15">
+      <c r="J15" s="3">
         <v>0</v>
       </c>
       <c r="K15">
@@ -1384,7 +1473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:24">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C16">
         <v>16</v>
       </c>
@@ -1406,7 +1495,7 @@
       <c r="I16">
         <v>0</v>
       </c>
-      <c r="J16">
+      <c r="J16" s="3">
         <v>0</v>
       </c>
       <c r="K16">
@@ -1431,7 +1520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C17">
         <v>17</v>
       </c>
@@ -1453,7 +1542,7 @@
       <c r="I17">
         <v>0</v>
       </c>
-      <c r="J17">
+      <c r="J17" s="3">
         <v>0</v>
       </c>
       <c r="K17">
@@ -1478,7 +1567,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>28</v>
       </c>
@@ -1503,8 +1592,8 @@
       <c r="I18">
         <v>0</v>
       </c>
-      <c r="J18">
-        <v>0</v>
+      <c r="J18" s="3">
+        <v>13</v>
       </c>
       <c r="K18">
         <v>0</v>
@@ -1525,10 +1614,10 @@
         <v>0</v>
       </c>
       <c r="Q18">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C19">
         <v>19</v>
       </c>
@@ -1550,7 +1639,7 @@
       <c r="I19">
         <v>0</v>
       </c>
-      <c r="J19">
+      <c r="J19" s="3">
         <v>0</v>
       </c>
       <c r="K19">
@@ -1575,7 +1664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:17">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C20">
         <v>20</v>
       </c>
@@ -1597,8 +1686,8 @@
       <c r="I20">
         <v>0</v>
       </c>
-      <c r="J20">
-        <v>0</v>
+      <c r="J20" s="3">
+        <v>5</v>
       </c>
       <c r="K20">
         <v>0</v>
@@ -1619,10 +1708,10 @@
         <v>0</v>
       </c>
       <c r="Q20">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>29</v>
       </c>
@@ -1647,8 +1736,8 @@
       <c r="I21">
         <v>0</v>
       </c>
-      <c r="J21">
-        <v>0</v>
+      <c r="J21" s="3">
+        <v>31</v>
       </c>
       <c r="K21">
         <v>0</v>
@@ -1669,10 +1758,10 @@
         <v>0</v>
       </c>
       <c r="Q21">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C22">
         <v>22</v>
       </c>
@@ -1694,7 +1783,7 @@
       <c r="I22">
         <v>0</v>
       </c>
-      <c r="J22">
+      <c r="J22" s="3">
         <v>0</v>
       </c>
       <c r="K22">
@@ -1719,7 +1808,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:17">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>23</v>
       </c>
@@ -1741,7 +1830,7 @@
       <c r="I23">
         <v>0</v>
       </c>
-      <c r="J23">
+      <c r="J23" s="3">
         <v>0</v>
       </c>
       <c r="K23">
@@ -1766,7 +1855,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:17">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C24">
         <v>24</v>
       </c>
@@ -1788,7 +1877,7 @@
       <c r="I24">
         <v>0</v>
       </c>
-      <c r="J24">
+      <c r="J24" s="3">
         <v>0</v>
       </c>
       <c r="K24">
@@ -1813,7 +1902,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C25">
         <v>25</v>
       </c>
@@ -1835,7 +1924,7 @@
       <c r="I25">
         <v>0</v>
       </c>
-      <c r="J25">
+      <c r="J25" s="3">
         <v>0</v>
       </c>
       <c r="K25">
@@ -1860,7 +1949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:17">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C26">
         <v>26</v>
       </c>
@@ -1882,7 +1971,7 @@
       <c r="I26">
         <v>0</v>
       </c>
-      <c r="J26">
+      <c r="J26" s="3">
         <v>0</v>
       </c>
       <c r="K26">
@@ -1907,7 +1996,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:17">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C27">
         <v>27</v>
       </c>
@@ -1929,7 +2018,7 @@
       <c r="I27">
         <v>0</v>
       </c>
-      <c r="J27">
+      <c r="J27" s="3">
         <v>0</v>
       </c>
       <c r="K27">
@@ -1954,7 +2043,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:17">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C28">
         <v>28</v>
       </c>
@@ -1976,8 +2065,8 @@
       <c r="I28">
         <v>0</v>
       </c>
-      <c r="J28">
-        <v>0</v>
+      <c r="J28" s="3">
+        <v>27</v>
       </c>
       <c r="K28">
         <v>0</v>
@@ -1998,10 +2087,10 @@
         <v>0</v>
       </c>
       <c r="Q28">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C29">
         <v>29</v>
       </c>
@@ -2023,8 +2112,8 @@
       <c r="I29">
         <v>0</v>
       </c>
-      <c r="J29">
-        <v>0</v>
+      <c r="J29" s="3">
+        <v>11</v>
       </c>
       <c r="K29">
         <v>0</v>
@@ -2045,10 +2134,10 @@
         <v>0</v>
       </c>
       <c r="Q29">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>24</v>
       </c>
@@ -2073,7 +2162,7 @@
       <c r="I30">
         <v>0</v>
       </c>
-      <c r="J30">
+      <c r="J30" s="3">
         <v>0</v>
       </c>
       <c r="K30">
@@ -2098,7 +2187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:17">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C31">
         <v>31</v>
       </c>
@@ -2120,7 +2209,7 @@
       <c r="I31">
         <v>0</v>
       </c>
-      <c r="J31">
+      <c r="J31" s="3">
         <v>0</v>
       </c>
       <c r="K31">
@@ -2145,7 +2234,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:17">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C32">
         <v>32</v>
       </c>
@@ -2167,7 +2256,7 @@
       <c r="I32">
         <v>0</v>
       </c>
-      <c r="J32">
+      <c r="J32" s="3">
         <v>0</v>
       </c>
       <c r="K32">
@@ -2192,7 +2281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="3:17">
+    <row r="33" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C33">
         <v>33</v>
       </c>
@@ -2214,7 +2303,7 @@
       <c r="I33">
         <v>0</v>
       </c>
-      <c r="J33">
+      <c r="J33" s="3">
         <v>0</v>
       </c>
       <c r="K33">
@@ -2239,7 +2328,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="3:17">
+    <row r="34" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C34">
         <v>34</v>
       </c>
@@ -2261,7 +2350,7 @@
       <c r="I34">
         <v>0</v>
       </c>
-      <c r="J34">
+      <c r="J34" s="3">
         <v>0</v>
       </c>
       <c r="K34">
@@ -2286,7 +2375,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="3:17">
+    <row r="35" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C35">
         <v>35</v>
       </c>
@@ -2308,7 +2397,7 @@
       <c r="I35">
         <v>0</v>
       </c>
-      <c r="J35">
+      <c r="J35" s="3">
         <v>0</v>
       </c>
       <c r="K35">
@@ -2333,7 +2422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="3:17">
+    <row r="36" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C36">
         <v>36</v>
       </c>
@@ -2355,7 +2444,7 @@
       <c r="I36">
         <v>0</v>
       </c>
-      <c r="J36">
+      <c r="J36" s="3">
         <v>0</v>
       </c>
       <c r="K36">
@@ -2380,7 +2469,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="3:17">
+    <row r="37" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C37">
         <v>37</v>
       </c>
@@ -2402,7 +2491,7 @@
       <c r="I37">
         <v>0</v>
       </c>
-      <c r="J37">
+      <c r="J37" s="3">
         <v>0</v>
       </c>
       <c r="K37">
@@ -2427,7 +2516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="3:17">
+    <row r="38" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C38">
         <v>38</v>
       </c>
@@ -2449,7 +2538,7 @@
       <c r="I38">
         <v>0</v>
       </c>
-      <c r="J38">
+      <c r="J38" s="3">
         <v>0</v>
       </c>
       <c r="K38">
@@ -2474,7 +2563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="3:17">
+    <row r="39" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C39">
         <v>39</v>
       </c>
@@ -2496,7 +2585,7 @@
       <c r="I39">
         <v>0</v>
       </c>
-      <c r="J39">
+      <c r="J39" s="3">
         <v>0</v>
       </c>
       <c r="K39">
@@ -2521,7 +2610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="3:17">
+    <row r="40" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C40">
         <v>40</v>
       </c>
@@ -2543,7 +2632,7 @@
       <c r="I40">
         <v>0</v>
       </c>
-      <c r="J40">
+      <c r="J40" s="3">
         <v>0</v>
       </c>
       <c r="K40">
@@ -2568,7 +2657,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="3:17">
+    <row r="41" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C41">
         <v>41</v>
       </c>
@@ -2590,7 +2679,7 @@
       <c r="I41">
         <v>0</v>
       </c>
-      <c r="J41">
+      <c r="J41" s="3">
         <v>0</v>
       </c>
       <c r="K41">
@@ -2615,7 +2704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="3:17">
+    <row r="42" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C42">
         <v>42</v>
       </c>
@@ -2637,7 +2726,7 @@
       <c r="I42">
         <v>0</v>
       </c>
-      <c r="J42">
+      <c r="J42" s="3">
         <v>0</v>
       </c>
       <c r="K42">
@@ -2662,7 +2751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="3:17">
+    <row r="43" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C43">
         <v>43</v>
       </c>
@@ -2684,7 +2773,7 @@
       <c r="I43">
         <v>0</v>
       </c>
-      <c r="J43">
+      <c r="J43" s="3">
         <v>0</v>
       </c>
       <c r="K43">
@@ -2709,7 +2798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="3:17">
+    <row r="44" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C44">
         <v>44</v>
       </c>
@@ -2731,7 +2820,7 @@
       <c r="I44">
         <v>0</v>
       </c>
-      <c r="J44">
+      <c r="J44" s="3">
         <v>0</v>
       </c>
       <c r="K44">
@@ -2756,7 +2845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="3:17">
+    <row r="45" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C45">
         <v>45</v>
       </c>
@@ -2778,7 +2867,7 @@
       <c r="I45">
         <v>0</v>
       </c>
-      <c r="J45">
+      <c r="J45" s="3">
         <v>0</v>
       </c>
       <c r="K45">
@@ -2803,7 +2892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="3:17">
+    <row r="46" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C46">
         <v>46</v>
       </c>
@@ -2825,7 +2914,7 @@
       <c r="I46">
         <v>0</v>
       </c>
-      <c r="J46">
+      <c r="J46" s="3">
         <v>0</v>
       </c>
       <c r="K46">
@@ -2850,7 +2939,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="3:17">
+    <row r="47" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C47">
         <v>47</v>
       </c>
@@ -2872,7 +2961,7 @@
       <c r="I47">
         <v>0</v>
       </c>
-      <c r="J47">
+      <c r="J47" s="3">
         <v>0</v>
       </c>
       <c r="K47">
@@ -2897,7 +2986,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="3:17">
+    <row r="48" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C48">
         <v>48</v>
       </c>
@@ -2919,7 +3008,7 @@
       <c r="I48">
         <v>0</v>
       </c>
-      <c r="J48">
+      <c r="J48" s="3">
         <v>0</v>
       </c>
       <c r="K48">
@@ -2944,7 +3033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:17">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>25</v>
       </c>
@@ -2972,7 +3061,7 @@
       <c r="I49">
         <v>0</v>
       </c>
-      <c r="J49">
+      <c r="J49" s="3">
         <v>0</v>
       </c>
       <c r="K49">
@@ -2997,7 +3086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:17">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C50">
         <v>50</v>
       </c>
@@ -3019,7 +3108,7 @@
       <c r="I50">
         <v>0</v>
       </c>
-      <c r="J50">
+      <c r="J50" s="3">
         <v>0</v>
       </c>
       <c r="K50">
@@ -3044,7 +3133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:17">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C51">
         <v>51</v>
       </c>
@@ -3066,7 +3155,7 @@
       <c r="I51">
         <v>0</v>
       </c>
-      <c r="J51">
+      <c r="J51" s="3">
         <v>0</v>
       </c>
       <c r="K51">
@@ -3091,7 +3180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:17">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C52">
         <v>52</v>
       </c>
@@ -3113,7 +3202,7 @@
       <c r="I52">
         <v>0</v>
       </c>
-      <c r="J52">
+      <c r="J52" s="3">
         <v>0</v>
       </c>
       <c r="K52">
@@ -3138,7 +3227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:17">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C53">
         <v>53</v>
       </c>
@@ -3160,7 +3249,7 @@
       <c r="I53">
         <v>0</v>
       </c>
-      <c r="J53">
+      <c r="J53" s="3">
         <v>0</v>
       </c>
       <c r="K53">
@@ -3185,7 +3274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:17">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C54">
         <v>54</v>
       </c>
@@ -3207,7 +3296,7 @@
       <c r="I54">
         <v>0</v>
       </c>
-      <c r="J54">
+      <c r="J54" s="3">
         <v>0</v>
       </c>
       <c r="K54">
@@ -3232,7 +3321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:17">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>31</v>
       </c>
@@ -3257,7 +3346,7 @@
       <c r="I55">
         <v>0</v>
       </c>
-      <c r="J55">
+      <c r="J55" s="3">
         <v>0</v>
       </c>
       <c r="K55">
@@ -3282,7 +3371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:17">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C56">
         <v>56</v>
       </c>
@@ -3304,7 +3393,7 @@
       <c r="I56">
         <v>0</v>
       </c>
-      <c r="J56">
+      <c r="J56" s="3">
         <v>0</v>
       </c>
       <c r="K56">
@@ -3329,7 +3418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:17">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C57">
         <v>57</v>
       </c>
@@ -3351,7 +3440,7 @@
       <c r="I57">
         <v>0</v>
       </c>
-      <c r="J57">
+      <c r="J57" s="3">
         <v>0</v>
       </c>
       <c r="K57">
@@ -3376,7 +3465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:17">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C58">
         <v>58</v>
       </c>
@@ -3398,7 +3487,7 @@
       <c r="I58">
         <v>0</v>
       </c>
-      <c r="J58">
+      <c r="J58" s="3">
         <v>0</v>
       </c>
       <c r="K58">
@@ -3423,7 +3512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:17">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C59">
         <v>59</v>
       </c>
@@ -3445,7 +3534,7 @@
       <c r="I59">
         <v>0</v>
       </c>
-      <c r="J59">
+      <c r="J59" s="3">
         <v>0</v>
       </c>
       <c r="K59">
@@ -3470,7 +3559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:17">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C60">
         <v>60</v>
       </c>
@@ -3492,7 +3581,7 @@
       <c r="I60">
         <v>0</v>
       </c>
-      <c r="J60">
+      <c r="J60" s="3">
         <v>0</v>
       </c>
       <c r="K60">
@@ -3517,7 +3606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:17">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C61">
         <v>61</v>
       </c>
@@ -3539,7 +3628,7 @@
       <c r="I61">
         <v>0</v>
       </c>
-      <c r="J61">
+      <c r="J61" s="3">
         <v>0</v>
       </c>
       <c r="K61">
@@ -3564,7 +3653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:17">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C62">
         <v>62</v>
       </c>
@@ -3586,7 +3675,7 @@
       <c r="I62">
         <v>0</v>
       </c>
-      <c r="J62">
+      <c r="J62" s="3">
         <v>0</v>
       </c>
       <c r="K62">
@@ -3611,7 +3700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:17">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C63">
         <v>63</v>
       </c>
@@ -3633,7 +3722,7 @@
       <c r="I63">
         <v>0</v>
       </c>
-      <c r="J63">
+      <c r="J63" s="3">
         <v>0</v>
       </c>
       <c r="K63">
@@ -3658,7 +3747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:17">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C64">
         <v>64</v>
       </c>
@@ -3680,7 +3769,7 @@
       <c r="I64">
         <v>0</v>
       </c>
-      <c r="J64">
+      <c r="J64" s="3">
         <v>0</v>
       </c>
       <c r="K64">
@@ -3705,7 +3794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:22">
+    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C65">
         <v>65</v>
       </c>
@@ -3727,7 +3816,7 @@
       <c r="I65">
         <v>0</v>
       </c>
-      <c r="J65">
+      <c r="J65" s="3">
         <v>0</v>
       </c>
       <c r="K65">
@@ -3752,7 +3841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:22">
+    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C66">
         <v>66</v>
       </c>
@@ -3774,7 +3863,7 @@
       <c r="I66">
         <v>0</v>
       </c>
-      <c r="J66">
+      <c r="J66" s="3">
         <v>0</v>
       </c>
       <c r="K66">
@@ -3799,7 +3888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:22">
+    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C67">
         <v>67</v>
       </c>
@@ -3821,7 +3910,7 @@
       <c r="I67">
         <v>0</v>
       </c>
-      <c r="J67">
+      <c r="J67" s="3">
         <v>0</v>
       </c>
       <c r="K67">
@@ -3846,7 +3935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:22">
+    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C68">
         <v>68</v>
       </c>
@@ -3868,7 +3957,7 @@
       <c r="I68">
         <v>0</v>
       </c>
-      <c r="J68">
+      <c r="J68" s="3">
         <v>0</v>
       </c>
       <c r="K68">
@@ -3893,7 +3982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:22">
+    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C69">
         <v>69</v>
       </c>
@@ -3915,7 +4004,7 @@
       <c r="I69">
         <v>0</v>
       </c>
-      <c r="J69">
+      <c r="J69" s="3">
         <v>0</v>
       </c>
       <c r="K69">
@@ -3940,7 +4029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:22">
+    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C70">
         <v>70</v>
       </c>
@@ -3962,7 +4051,7 @@
       <c r="I70">
         <v>0</v>
       </c>
-      <c r="J70">
+      <c r="J70" s="3">
         <v>0</v>
       </c>
       <c r="K70">
@@ -3987,7 +4076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:22">
+    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C71">
         <v>71</v>
       </c>
@@ -4009,7 +4098,7 @@
       <c r="I71">
         <v>0</v>
       </c>
-      <c r="J71">
+      <c r="J71" s="3">
         <v>0</v>
       </c>
       <c r="K71">
@@ -4034,7 +4123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:22">
+    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C72">
         <v>72</v>
       </c>
@@ -4056,7 +4145,7 @@
       <c r="I72">
         <v>0</v>
       </c>
-      <c r="J72">
+      <c r="J72" s="3">
         <v>0</v>
       </c>
       <c r="K72">
@@ -4081,7 +4170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:22">
+    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C73">
         <v>73</v>
       </c>
@@ -4103,7 +4192,7 @@
       <c r="I73">
         <v>0</v>
       </c>
-      <c r="J73">
+      <c r="J73" s="3">
         <v>0</v>
       </c>
       <c r="K73">
@@ -4128,7 +4217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:22">
+    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C74">
         <v>74</v>
       </c>
@@ -4150,7 +4239,7 @@
       <c r="I74">
         <v>0</v>
       </c>
-      <c r="J74">
+      <c r="J74" s="3">
         <v>0</v>
       </c>
       <c r="K74">
@@ -4175,7 +4264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:22">
+    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>26</v>
       </c>
@@ -4200,7 +4289,7 @@
       <c r="I75">
         <v>0</v>
       </c>
-      <c r="J75">
+      <c r="J75" s="3">
         <v>0</v>
       </c>
       <c r="K75">

</xml_diff>